<commit_message>
Muchas cosas que no subi antes de irme de vacaciones
</commit_message>
<xml_diff>
--- a/5° Año/1° Semestre/Modelos y simulacion/Mario Molina Estocastica/Pyhton/Soria - football - TP3.xlsx
+++ b/5° Año/1° Semestre/Modelos y simulacion/Mario Molina Estocastica/Pyhton/Soria - football - TP3.xlsx
@@ -1878,10 +1878,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="F11" t="n">
-        <v>15.9995314167929</v>
+        <v>15.87300763282674</v>
       </c>
       <c r="G11" t="n">
-        <v>4.413453635429168</v>
+        <v>4.404014838238158</v>
       </c>
       <c r="H11" t="n">
         <v>11.49990257669732</v>
@@ -1890,10 +1890,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="J11" t="n">
-        <v>15.97585228619147</v>
+        <v>15.8852722069711</v>
       </c>
       <c r="K11" t="n">
-        <v>4.442223953928247</v>
+        <v>4.373224116456633</v>
       </c>
       <c r="L11" t="n">
         <v>11.49990257669732</v>
@@ -1902,10 +1902,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="N11" t="n">
-        <v>15.87567383367852</v>
+        <v>15.90920571684925</v>
       </c>
       <c r="O11" t="n">
-        <v>4.434992865580413</v>
+        <v>4.384740382283893</v>
       </c>
       <c r="P11" t="n">
         <v>11.49990257669732</v>
@@ -1914,10 +1914,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="R11" t="n">
-        <v>15.88872321043358</v>
+        <v>15.90916823392689</v>
       </c>
       <c r="S11" t="n">
-        <v>4.396518385267536</v>
+        <v>4.376359355128463</v>
       </c>
       <c r="T11" t="n">
         <v>11.49990257669732</v>
@@ -1926,10 +1926,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="V11" t="n">
-        <v>15.93169133391581</v>
+        <v>15.95637366816711</v>
       </c>
       <c r="W11" t="n">
-        <v>4.389532245362886</v>
+        <v>4.416070547320406</v>
       </c>
       <c r="X11" t="n">
         <v>11.49990257669732</v>
@@ -1938,10 +1938,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="Z11" t="n">
-        <v>15.90500732956037</v>
+        <v>15.92706851935741</v>
       </c>
       <c r="AA11" t="n">
-        <v>4.392078244489719</v>
+        <v>4.467061194628723</v>
       </c>
       <c r="AB11" t="n">
         <v>11.49990257669732</v>
@@ -1950,10 +1950,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="AD11" t="n">
-        <v>15.84872201452782</v>
+        <v>15.91152060688728</v>
       </c>
       <c r="AE11" t="n">
-        <v>4.413318486852413</v>
+        <v>4.39369613675494</v>
       </c>
       <c r="AF11" t="n">
         <v>11.49990257669732</v>
@@ -1962,10 +1962,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="AH11" t="n">
-        <v>15.97839796573462</v>
+        <v>15.99858946220556</v>
       </c>
       <c r="AI11" t="n">
-        <v>4.318781750285746</v>
+        <v>4.344421483087142</v>
       </c>
       <c r="AJ11" t="n">
         <v>11.49990257669732</v>
@@ -1974,10 +1974,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="AL11" t="n">
-        <v>15.89647672936215</v>
+        <v>15.86795641066724</v>
       </c>
       <c r="AM11" t="n">
-        <v>4.396394980239276</v>
+        <v>4.389060559742402</v>
       </c>
       <c r="AN11" t="n">
         <v>11.49990257669732</v>
@@ -1986,10 +1986,10 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="AP11" t="n">
-        <v>15.90990257669732</v>
+        <v>15.88430792523039</v>
       </c>
       <c r="AQ11" t="n">
-        <v>4.389532245362886</v>
+        <v>4.351394154023185</v>
       </c>
       <c r="AR11" t="n">
         <v>11.49990257669732</v>
@@ -2012,10 +2012,10 @@
         <v>0.8</v>
       </c>
       <c r="F12" t="n">
-        <v>17.94655604995042</v>
+        <v>17.56698469805195</v>
       </c>
       <c r="G12" t="n">
-        <v>4.949022220602052</v>
+        <v>4.920705829029022</v>
       </c>
       <c r="H12" t="n">
         <v>12.28766952966369</v>
@@ -2024,10 +2024,10 @@
         <v>0.8</v>
       </c>
       <c r="J12" t="n">
-        <v>17.87551865814614</v>
+        <v>17.60377842048505</v>
       </c>
       <c r="K12" t="n">
-        <v>5.035333176099289</v>
+        <v>4.828333663684448</v>
       </c>
       <c r="L12" t="n">
         <v>12.28766952966369</v>
@@ -2036,10 +2036,10 @@
         <v>0.8</v>
       </c>
       <c r="N12" t="n">
-        <v>17.57498330060729</v>
+        <v>17.67557895011948</v>
       </c>
       <c r="O12" t="n">
-        <v>5.013639911055787</v>
+        <v>4.862882461166228</v>
       </c>
       <c r="P12" t="n">
         <v>12.28766952966369</v>
@@ -2048,10 +2048,10 @@
         <v>0.8</v>
       </c>
       <c r="R12" t="n">
-        <v>17.61413143087246</v>
+        <v>17.67546650135241</v>
       </c>
       <c r="S12" t="n">
-        <v>4.898216470117157</v>
+        <v>4.837739379699936</v>
       </c>
       <c r="T12" t="n">
         <v>12.28766952966369</v>
@@ -2060,10 +2060,10 @@
         <v>0.8</v>
       </c>
       <c r="V12" t="n">
-        <v>17.74303580131916</v>
+        <v>17.81708280407307</v>
       </c>
       <c r="W12" t="n">
-        <v>4.877258050403207</v>
+        <v>4.956872956275768</v>
       </c>
       <c r="X12" t="n">
         <v>12.28766952966369</v>
@@ -2072,10 +2072,10 @@
         <v>0.8</v>
       </c>
       <c r="Z12" t="n">
-        <v>17.66298378825283</v>
+        <v>17.72916735764397</v>
       </c>
       <c r="AA12" t="n">
-        <v>4.884896047783704</v>
+        <v>5.109844898200716</v>
       </c>
       <c r="AB12" t="n">
         <v>12.28766952966369</v>
@@ -2084,10 +2084,10 @@
         <v>0.8</v>
       </c>
       <c r="AD12" t="n">
-        <v>17.49412784315518</v>
+        <v>17.68252362023357</v>
       </c>
       <c r="AE12" t="n">
-        <v>4.948616774871788</v>
+        <v>4.889749724579368</v>
       </c>
       <c r="AF12" t="n">
         <v>12.28766952966369</v>
@@ -2096,10 +2096,10 @@
         <v>0.8</v>
       </c>
       <c r="AH12" t="n">
-        <v>17.88315569677558</v>
+        <v>17.94373018618841</v>
       </c>
       <c r="AI12" t="n">
-        <v>4.665006565171787</v>
+        <v>4.741925763575976</v>
       </c>
       <c r="AJ12" t="n">
         <v>12.28766952966369</v>
@@ -2108,10 +2108,10 @@
         <v>0.8</v>
       </c>
       <c r="AL12" t="n">
-        <v>17.65081783499334</v>
+        <v>17.55183103157346</v>
       </c>
       <c r="AM12" t="n">
-        <v>4.890983520155987</v>
+        <v>4.875842993541755</v>
       </c>
       <c r="AN12" t="n">
         <v>12.28766952966369</v>
@@ -2120,10 +2120,10 @@
         <v>0.8</v>
       </c>
       <c r="AP12" t="n">
-        <v>17.67766952966369</v>
+        <v>17.60088557526291</v>
       </c>
       <c r="AQ12" t="n">
-        <v>4.877258050403207</v>
+        <v>4.762843776384104</v>
       </c>
       <c r="AR12" t="n">
         <v>12.28766952966369</v>
@@ -2146,10 +2146,10 @@
         <v>0.9</v>
       </c>
       <c r="F13" t="n">
-        <v>19.98320952320353</v>
+        <v>19.22406681940658</v>
       </c>
       <c r="G13" t="n">
-        <v>5.508512195841217</v>
+        <v>5.451879412695158</v>
       </c>
       <c r="H13" t="n">
         <v>12.97743648263006</v>
@@ -2158,10 +2158,10 @@
         <v>0.9</v>
       </c>
       <c r="J13" t="n">
-        <v>19.84113473959497</v>
+        <v>19.29765426427277</v>
       </c>
       <c r="K13" t="n">
-        <v>5.681134106835692</v>
+        <v>5.267135082006009</v>
       </c>
       <c r="L13" t="n">
         <v>12.97743648263006</v>
@@ -2170,10 +2170,10 @@
         <v>0.9</v>
       </c>
       <c r="N13" t="n">
-        <v>19.24006402451725</v>
+        <v>19.44125532354164</v>
       </c>
       <c r="O13" t="n">
-        <v>5.637747576748687</v>
+        <v>5.336232676969569</v>
       </c>
       <c r="P13" t="n">
         <v>12.97743648263006</v>
@@ -2182,10 +2182,10 @@
         <v>0.9</v>
       </c>
       <c r="R13" t="n">
-        <v>19.3183602850476</v>
+        <v>19.44103042600751</v>
       </c>
       <c r="S13" t="n">
-        <v>5.406900694871428</v>
+        <v>5.285946514036986</v>
       </c>
       <c r="T13" t="n">
         <v>12.97743648263006</v>
@@ -2194,10 +2194,10 @@
         <v>0.9</v>
       </c>
       <c r="V13" t="n">
-        <v>19.57616902594101</v>
+        <v>19.72426303144882</v>
       </c>
       <c r="W13" t="n">
-        <v>5.364983855443528</v>
+        <v>5.52421366718865</v>
       </c>
       <c r="X13" t="n">
         <v>12.97743648263006</v>
@@ -2206,10 +2206,10 @@
         <v>0.9</v>
       </c>
       <c r="Z13" t="n">
-        <v>19.41606499980834</v>
+        <v>19.54843213859062</v>
       </c>
       <c r="AA13" t="n">
-        <v>5.380259850204522</v>
+        <v>5.830157551038546</v>
       </c>
       <c r="AB13" t="n">
         <v>12.97743648263006</v>
@@ -2218,10 +2218,10 @@
         <v>0.9</v>
       </c>
       <c r="AD13" t="n">
-        <v>19.07835310961304</v>
+        <v>19.45514466376983</v>
       </c>
       <c r="AE13" t="n">
-        <v>5.507701304380689</v>
+        <v>5.389967203795851</v>
       </c>
       <c r="AF13" t="n">
         <v>12.97743648263006</v>
@@ -2230,10 +2230,10 @@
         <v>0.9</v>
       </c>
       <c r="AH13" t="n">
-        <v>19.85640881685385</v>
+        <v>19.97755779567951</v>
       </c>
       <c r="AI13" t="n">
-        <v>4.940480884980687</v>
+        <v>5.094319281789065</v>
       </c>
       <c r="AJ13" t="n">
         <v>12.97743648263006</v>
@@ -2242,10 +2242,10 @@
         <v>0.9</v>
       </c>
       <c r="AL13" t="n">
-        <v>19.40515894062453</v>
+        <v>19.19375948644961</v>
       </c>
       <c r="AM13" t="n">
-        <v>5.385572060072698</v>
+        <v>5.362153741720625</v>
       </c>
       <c r="AN13" t="n">
         <v>12.97743648263006</v>
@@ -2254,10 +2254,10 @@
         <v>0.9</v>
       </c>
       <c r="AP13" t="n">
-        <v>19.44543648263005</v>
+        <v>19.29186857382851</v>
       </c>
       <c r="AQ13" t="n">
-        <v>5.364983855443528</v>
+        <v>5.136155307405321</v>
       </c>
       <c r="AR13" t="n">
         <v>12.97743648263006</v>
@@ -2280,10 +2280,10 @@
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>22.10949183655221</v>
+        <v>20.84425399689063</v>
       </c>
       <c r="G14" t="n">
-        <v>6.091923561146663</v>
+        <v>5.997535589236565</v>
       </c>
       <c r="H14" t="n">
         <v>13.56920343559642</v>
@@ -2292,10 +2292,10 @@
         <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>21.87270053053794</v>
+        <v>20.96689973833428</v>
       </c>
       <c r="K14" t="n">
-        <v>6.379626746137455</v>
+        <v>5.689628371421318</v>
       </c>
       <c r="L14" t="n">
         <v>13.56920343559642</v>
@@ -2304,10 +2304,10 @@
         <v>1</v>
       </c>
       <c r="N14" t="n">
-        <v>20.87091600540842</v>
+        <v>21.20623483711573</v>
       </c>
       <c r="O14" t="n">
-        <v>6.307315862659115</v>
+        <v>5.804791029693917</v>
       </c>
       <c r="P14" t="n">
         <v>13.56920343559642</v>
@@ -2316,10 +2316,10 @@
         <v>1</v>
       </c>
       <c r="R14" t="n">
-        <v>21.001409772959</v>
+        <v>21.20586000789218</v>
       </c>
       <c r="S14" t="n">
-        <v>5.922571059530349</v>
+        <v>5.720980758139612</v>
       </c>
       <c r="T14" t="n">
         <v>13.56920343559642</v>
@@ -2328,10 +2328,10 @@
         <v>1</v>
       </c>
       <c r="V14" t="n">
-        <v>21.43109100778134</v>
+        <v>21.67791435029436</v>
       </c>
       <c r="W14" t="n">
-        <v>5.852709660483849</v>
+        <v>6.118092680059052</v>
       </c>
       <c r="X14" t="n">
         <v>13.56920343559642</v>
@@ -2340,10 +2340,10 @@
         <v>1</v>
       </c>
       <c r="Z14" t="n">
-        <v>21.16425096422691</v>
+        <v>21.38486286219737</v>
       </c>
       <c r="AA14" t="n">
-        <v>5.878169651752173</v>
+        <v>6.627999153142213</v>
       </c>
       <c r="AB14" t="n">
         <v>13.56920343559642</v>
@@ -2352,10 +2352,10 @@
         <v>1</v>
       </c>
       <c r="AD14" t="n">
-        <v>20.60139781390139</v>
+        <v>21.22938373749604</v>
       </c>
       <c r="AE14" t="n">
-        <v>6.090572075379116</v>
+        <v>5.894348574404387</v>
       </c>
       <c r="AF14" t="n">
         <v>13.56920343559642</v>
@@ -2364,10 +2364,10 @@
         <v>1</v>
       </c>
       <c r="AH14" t="n">
-        <v>21.89815732596941</v>
+        <v>22.10007229067885</v>
       </c>
       <c r="AI14" t="n">
-        <v>5.145204709712447</v>
+        <v>5.401602037726411</v>
       </c>
       <c r="AJ14" t="n">
         <v>13.56920343559642</v>
@@ -2376,10 +2376,10 @@
         <v>1</v>
       </c>
       <c r="AL14" t="n">
-        <v>21.15950004625573</v>
+        <v>20.79374177529568</v>
       </c>
       <c r="AM14" t="n">
-        <v>5.880160599989408</v>
+        <v>5.84799280427901</v>
       </c>
       <c r="AN14" t="n">
         <v>13.56920343559642</v>
@@ -2388,10 +2388,10 @@
         <v>1</v>
       </c>
       <c r="AP14" t="n">
-        <v>21.21320343559642</v>
+        <v>20.95725692092718</v>
       </c>
       <c r="AQ14" t="n">
-        <v>5.852709660483849</v>
+        <v>5.471328747086837</v>
       </c>
       <c r="AR14" t="n">
         <v>13.56920343559642</v>
@@ -2414,10 +2414,10 @@
         <v>1.1</v>
       </c>
       <c r="F15" t="n">
-        <v>24.32540298999648</v>
+        <v>22.4275462305041</v>
       </c>
       <c r="G15" t="n">
-        <v>6.69925631651839</v>
+        <v>6.557674358653244</v>
       </c>
       <c r="H15" t="n">
         <v>14.06297038856279</v>
@@ -2426,10 +2426,10 @@
         <v>1.1</v>
       </c>
       <c r="J15" t="n">
-        <v>23.97021603097507</v>
+        <v>22.61151484266958</v>
       </c>
       <c r="K15" t="n">
-        <v>7.130811094004579</v>
+        <v>6.095813531930373</v>
       </c>
       <c r="L15" t="n">
         <v>14.06297038856279</v>
@@ -2438,10 +2438,10 @@
         <v>1.1</v>
       </c>
       <c r="N15" t="n">
-        <v>22.46753924328078</v>
+        <v>22.97051749084175</v>
       </c>
       <c r="O15" t="n">
-        <v>7.022344768787069</v>
+        <v>6.268557519339272</v>
       </c>
       <c r="P15" t="n">
         <v>14.06297038856279</v>
@@ -2450,10 +2450,10 @@
         <v>1.1</v>
       </c>
       <c r="R15" t="n">
-        <v>22.66327989460666</v>
+        <v>22.96995524700642</v>
       </c>
       <c r="S15" t="n">
-        <v>6.44522756409392</v>
+        <v>6.142842112007815</v>
       </c>
       <c r="T15" t="n">
         <v>14.06297038856279</v>
@@ -2462,10 +2462,10 @@
         <v>1.1</v>
       </c>
       <c r="V15" t="n">
-        <v>23.30780174684017</v>
+        <v>23.6780367606097</v>
       </c>
       <c r="W15" t="n">
-        <v>6.34043546552417</v>
+        <v>6.738509994886974</v>
       </c>
       <c r="X15" t="n">
         <v>14.06297038856279</v>
@@ -2474,10 +2474,10 @@
         <v>1.1</v>
       </c>
       <c r="Z15" t="n">
-        <v>22.90754168150852</v>
+        <v>23.23845952846422</v>
       </c>
       <c r="AA15" t="n">
-        <v>6.378625452426656</v>
+        <v>7.503369704511716</v>
       </c>
       <c r="AB15" t="n">
         <v>14.06297038856279</v>
@@ -2486,10 +2486,10 @@
         <v>1.1</v>
       </c>
       <c r="AD15" t="n">
-        <v>22.06326195602024</v>
+        <v>23.00524084141222</v>
       </c>
       <c r="AE15" t="n">
-        <v>6.697229087867071</v>
+        <v>6.402893836404977</v>
       </c>
       <c r="AF15" t="n">
         <v>14.06297038856279</v>
@@ -2498,10 +2498,10 @@
         <v>1.1</v>
       </c>
       <c r="AH15" t="n">
-        <v>24.00840122412227</v>
+        <v>24.31127367118643</v>
       </c>
       <c r="AI15" t="n">
-        <v>5.279178039367067</v>
+        <v>5.663774031388013</v>
       </c>
       <c r="AJ15" t="n">
         <v>14.06297038856279</v>
@@ -2510,10 +2510,10 @@
         <v>1.1</v>
       </c>
       <c r="AL15" t="n">
-        <v>22.91384115188692</v>
+        <v>22.35177789811168</v>
       </c>
       <c r="AM15" t="n">
-        <v>6.374749139906119</v>
+        <v>6.333360181216912</v>
       </c>
       <c r="AN15" t="n">
         <v>14.06297038856279</v>
@@ -2522,10 +2522,10 @@
         <v>1.1</v>
       </c>
       <c r="AP15" t="n">
-        <v>22.98097038856279</v>
+        <v>22.59705061655892</v>
       </c>
       <c r="AQ15" t="n">
-        <v>6.34043546552417</v>
+        <v>5.768364095428651</v>
       </c>
       <c r="AR15" t="n">
         <v>14.06297038856279</v>
@@ -2548,10 +2548,10 @@
         <v>1.2</v>
       </c>
       <c r="F16" t="n">
-        <v>26.63094298353632</v>
+        <v>23.97394352024699</v>
       </c>
       <c r="G16" t="n">
-        <v>7.3305104619564</v>
+        <v>7.132295720945196</v>
       </c>
       <c r="H16" t="n">
         <v>14.45873734152916</v>
@@ -2560,10 +2560,10 @@
         <v>1.2</v>
       </c>
       <c r="J16" t="n">
-        <v>26.13368124090636</v>
+        <v>24.23149957727867</v>
       </c>
       <c r="K16" t="n">
-        <v>7.934687150437064</v>
+        <v>6.485690563533176</v>
       </c>
       <c r="L16" t="n">
         <v>14.45873734152916</v>
@@ -2572,10 +2572,10 @@
         <v>1.2</v>
       </c>
       <c r="N16" t="n">
-        <v>24.02993373813435</v>
+        <v>24.73410328471971</v>
       </c>
       <c r="O16" t="n">
-        <v>7.78283429513255</v>
+        <v>6.727532145905634</v>
       </c>
       <c r="P16" t="n">
         <v>14.45873734152916</v>
@@ -2584,10 +2584,10 @@
         <v>1.2</v>
       </c>
       <c r="R16" t="n">
-        <v>24.30397064999058</v>
+        <v>24.73331614335024</v>
       </c>
       <c r="S16" t="n">
-        <v>6.974870208562141</v>
+        <v>6.551530575641594</v>
       </c>
       <c r="T16" t="n">
         <v>14.45873734152916</v>
@@ -2596,10 +2596,10 @@
         <v>1.2</v>
       </c>
       <c r="V16" t="n">
-        <v>25.20630124311748</v>
+        <v>25.72463026239483</v>
       </c>
       <c r="W16" t="n">
-        <v>6.828161270564491</v>
+        <v>7.385465611672418</v>
       </c>
       <c r="X16" t="n">
         <v>14.45873734152916</v>
@@ -2608,10 +2608,10 @@
         <v>1.2</v>
       </c>
       <c r="Z16" t="n">
-        <v>24.64593715165318</v>
+        <v>25.10922213739115</v>
       </c>
       <c r="AA16" t="n">
-        <v>6.881627252227971</v>
+        <v>8.456269205147056</v>
       </c>
       <c r="AB16" t="n">
         <v>14.45873734152916</v>
@@ -2620,10 +2620,10 @@
         <v>1.2</v>
       </c>
       <c r="AD16" t="n">
-        <v>23.46394553596959</v>
+        <v>24.78271597551835</v>
       </c>
       <c r="AE16" t="n">
-        <v>7.327672341844552</v>
+        <v>6.915602989797621</v>
       </c>
       <c r="AF16" t="n">
         <v>14.45873734152916</v>
@@ -2632,10 +2632,10 @@
         <v>1.2</v>
       </c>
       <c r="AH16" t="n">
-        <v>26.18714051131244</v>
+        <v>26.61116193720225</v>
       </c>
       <c r="AI16" t="n">
-        <v>5.342400873944547</v>
+        <v>5.880835262773871</v>
       </c>
       <c r="AJ16" t="n">
         <v>14.45873734152916</v>
@@ -2644,10 +2644,10 @@
         <v>1.2</v>
       </c>
       <c r="AL16" t="n">
-        <v>24.66818225751812</v>
+        <v>23.86786785489761</v>
       </c>
       <c r="AM16" t="n">
-        <v>6.86933767982283</v>
+        <v>6.818255872534329</v>
       </c>
       <c r="AN16" t="n">
         <v>14.45873734152916</v>
@@ -2656,10 +2656,10 @@
         <v>1.2</v>
       </c>
       <c r="AP16" t="n">
-        <v>24.74873734152916</v>
+        <v>24.21124966072374</v>
       </c>
       <c r="AQ16" t="n">
-        <v>6.828161270564491</v>
+        <v>6.027261352430764</v>
       </c>
       <c r="AR16" t="n">
         <v>14.45873734152916</v>
@@ -2682,10 +2682,10 @@
         <v>1.3</v>
       </c>
       <c r="F17" t="n">
-        <v>29.02611181717174</v>
+        <v>25.4834458661193</v>
       </c>
       <c r="G17" t="n">
-        <v>7.98568599746069</v>
+        <v>7.721399676112419</v>
       </c>
       <c r="H17" t="n">
         <v>14.75650429449553</v>
@@ -2694,10 +2694,10 @@
         <v>1.3</v>
       </c>
       <c r="J17" t="n">
-        <v>28.36309616033179</v>
+        <v>25.82685394216153</v>
       </c>
       <c r="K17" t="n">
-        <v>8.791254915434909</v>
+        <v>6.859259466229725</v>
       </c>
       <c r="L17" t="n">
         <v>14.75650429449553</v>
@@ -2706,10 +2706,10 @@
         <v>1.3</v>
       </c>
       <c r="N17" t="n">
-        <v>25.55809948996911</v>
+        <v>26.49699221874959</v>
       </c>
       <c r="O17" t="n">
-        <v>8.588784441695557</v>
+        <v>7.181714909393003</v>
       </c>
       <c r="P17" t="n">
         <v>14.75650429449553</v>
@@ -2718,10 +2718,10 @@
         <v>1.3</v>
       </c>
       <c r="R17" t="n">
-        <v>25.92348203911076</v>
+        <v>26.49594269692364</v>
       </c>
       <c r="S17" t="n">
-        <v>7.511498992935012</v>
+        <v>6.94704614904095</v>
       </c>
       <c r="T17" t="n">
         <v>14.75650429449553</v>
@@ -2730,10 +2730,10 @@
         <v>1.3</v>
       </c>
       <c r="V17" t="n">
-        <v>27.12658949661329</v>
+        <v>27.81769485564976</v>
       </c>
       <c r="W17" t="n">
-        <v>7.315887075604811</v>
+        <v>8.058959530415381</v>
       </c>
       <c r="X17" t="n">
         <v>14.75650429449553</v>
@@ -2742,10 +2742,10 @@
         <v>1.3</v>
       </c>
       <c r="Z17" t="n">
-        <v>26.37943737466089</v>
+        <v>26.99715068897819</v>
       </c>
       <c r="AA17" t="n">
-        <v>7.387175051156118</v>
+        <v>9.486697655048232</v>
       </c>
       <c r="AB17" t="n">
         <v>14.75650429449553</v>
@@ -2754,10 +2754,10 @@
         <v>1.3</v>
       </c>
       <c r="AD17" t="n">
-        <v>24.80344855374944</v>
+        <v>26.56180913981445</v>
       </c>
       <c r="AE17" t="n">
-        <v>7.981901837311561</v>
+        <v>7.43247603458232</v>
       </c>
       <c r="AF17" t="n">
         <v>14.75650429449553</v>
@@ -2766,10 +2766,10 @@
         <v>1.3</v>
       </c>
       <c r="AH17" t="n">
-        <v>28.43437518753989</v>
+        <v>28.99973708872632</v>
       </c>
       <c r="AI17" t="n">
-        <v>5.334873213444886</v>
+        <v>6.052785731883986</v>
       </c>
       <c r="AJ17" t="n">
         <v>14.75650429449553</v>
@@ -2778,10 +2778,10 @@
         <v>1.3</v>
       </c>
       <c r="AL17" t="n">
-        <v>26.42252336314931</v>
+        <v>25.34201164565346</v>
       </c>
       <c r="AM17" t="n">
-        <v>7.363926219739541</v>
+        <v>7.302679878231263</v>
       </c>
       <c r="AN17" t="n">
         <v>14.75650429449553</v>
@@ -2790,10 +2790,10 @@
         <v>1.3</v>
       </c>
       <c r="AP17" t="n">
-        <v>26.51650429449553</v>
+        <v>25.79985405342164</v>
       </c>
       <c r="AQ17" t="n">
-        <v>7.315887075604811</v>
+        <v>6.248020518093176</v>
       </c>
       <c r="AR17" t="n">
         <v>14.75650429449553</v>
@@ -2816,10 +2816,10 @@
         <v>1.4</v>
       </c>
       <c r="F18" t="n">
-        <v>31.51090949090274</v>
+        <v>26.95605326812104</v>
       </c>
       <c r="G18" t="n">
-        <v>8.664782923031263</v>
+        <v>8.324986224154914</v>
       </c>
       <c r="H18" t="n">
         <v>14.9562712474619</v>
@@ -2828,10 +2828,10 @@
         <v>1.4</v>
       </c>
       <c r="J18" t="n">
-        <v>30.65846078925138</v>
+        <v>27.39757793731819</v>
       </c>
       <c r="K18" t="n">
-        <v>9.700514388998114</v>
+        <v>7.216520240020021</v>
       </c>
       <c r="L18" t="n">
         <v>14.9562712474619</v>
@@ -2840,10 +2840,10 @@
         <v>1.4</v>
       </c>
       <c r="N18" t="n">
-        <v>27.05203649878507</v>
+        <v>28.25918429293141</v>
       </c>
       <c r="O18" t="n">
-        <v>9.440195208476091</v>
+        <v>7.631105809801379</v>
       </c>
       <c r="P18" t="n">
         <v>14.9562712474619</v>
@@ -2852,10 +2852,10 @@
         <v>1.4</v>
       </c>
       <c r="R18" t="n">
-        <v>27.52181406196719</v>
+        <v>28.25783490772661</v>
       </c>
       <c r="S18" t="n">
-        <v>8.055113917212532</v>
+        <v>7.329388832205882</v>
       </c>
       <c r="T18" t="n">
         <v>14.9562712474619</v>
@@ -2864,10 +2864,10 @@
         <v>1.4</v>
       </c>
       <c r="V18" t="n">
-        <v>29.06866650732759</v>
+        <v>29.95723054037448</v>
       </c>
       <c r="W18" t="n">
-        <v>7.803612880645132</v>
+        <v>8.758991751115865</v>
       </c>
       <c r="X18" t="n">
         <v>14.9562712474619</v>
@@ -2876,10 +2876,10 @@
         <v>1.4</v>
       </c>
       <c r="Z18" t="n">
-        <v>28.10804235053164</v>
+        <v>28.90224518322531</v>
       </c>
       <c r="AA18" t="n">
-        <v>7.895268849211099</v>
+        <v>10.59465505421525</v>
       </c>
       <c r="AB18" t="n">
         <v>14.9562712474619</v>
@@ -2888,10 +2888,10 @@
         <v>1.4</v>
       </c>
       <c r="AD18" t="n">
-        <v>26.08177100935978</v>
+        <v>28.34252033430052</v>
       </c>
       <c r="AE18" t="n">
-        <v>8.659917574268096</v>
+        <v>7.953512970759071</v>
       </c>
       <c r="AF18" t="n">
         <v>14.9562712474619</v>
@@ -2900,10 +2900,10 @@
         <v>1.4</v>
       </c>
       <c r="AH18" t="n">
-        <v>30.75010525280465</v>
+        <v>31.47699912575862</v>
       </c>
       <c r="AI18" t="n">
-        <v>5.256595057868085</v>
+        <v>6.179625438718357</v>
       </c>
       <c r="AJ18" t="n">
         <v>14.9562712474619</v>
@@ -2912,10 +2912,10 @@
         <v>1.4</v>
       </c>
       <c r="AL18" t="n">
-        <v>28.17686446878051</v>
+        <v>26.77420927037923</v>
       </c>
       <c r="AM18" t="n">
-        <v>7.858514759656251</v>
+        <v>7.786632198307713</v>
       </c>
       <c r="AN18" t="n">
         <v>14.9562712474619</v>
@@ -2924,10 +2924,10 @@
         <v>1.4</v>
       </c>
       <c r="AP18" t="n">
-        <v>28.2842712474619</v>
+        <v>27.36286379465261</v>
       </c>
       <c r="AQ18" t="n">
-        <v>7.803612880645132</v>
+        <v>6.430641592415887</v>
       </c>
       <c r="AR18" t="n">
         <v>14.9562712474619</v>
@@ -2950,10 +2950,10 @@
         <v>1.5</v>
       </c>
       <c r="F19" t="n">
-        <v>34.08533600472931</v>
+        <v>28.39176572625219</v>
       </c>
       <c r="G19" t="n">
-        <v>9.367801238668116</v>
+        <v>8.943055365072681</v>
       </c>
       <c r="H19" t="n">
         <v>15.05803820042827</v>
@@ -2962,10 +2962,10 @@
         <v>1.5</v>
       </c>
       <c r="J19" t="n">
-        <v>33.01977512766511</v>
+        <v>28.94367156274863</v>
       </c>
       <c r="K19" t="n">
-        <v>10.66246557112668</v>
+        <v>7.557472884904064</v>
       </c>
       <c r="L19" t="n">
         <v>15.05803820042827</v>
@@ -2974,10 +2974,10 @@
         <v>1.5</v>
       </c>
       <c r="N19" t="n">
-        <v>28.51174476458224</v>
+        <v>30.02137636711322</v>
       </c>
       <c r="O19" t="n">
-        <v>10.33706659547415</v>
+        <v>8.080496710209754</v>
       </c>
       <c r="P19" t="n">
         <v>15.05803820042827</v>
@@ -2986,10 +2986,10 @@
         <v>1.5</v>
       </c>
       <c r="R19" t="n">
-        <v>29.09896671855989</v>
+        <v>30.01899277575916</v>
       </c>
       <c r="S19" t="n">
-        <v>8.605714981394703</v>
+        <v>7.69855862513639</v>
       </c>
       <c r="T19" t="n">
         <v>15.05803820042827</v>
@@ -2998,10 +2998,10 @@
         <v>1.5</v>
       </c>
       <c r="V19" t="n">
-        <v>31.03253227526039</v>
+        <v>32.14323731656899</v>
       </c>
       <c r="W19" t="n">
-        <v>8.291338685685453</v>
+        <v>9.485562273773869</v>
       </c>
       <c r="X19" t="n">
         <v>15.05803820042827</v>
@@ -3010,10 +3010,10 @@
         <v>1.5</v>
       </c>
       <c r="Z19" t="n">
-        <v>29.83175207926545</v>
+        <v>30.80733967747244</v>
       </c>
       <c r="AA19" t="n">
-        <v>8.405908646392911</v>
+        <v>11.70261245338226</v>
       </c>
       <c r="AB19" t="n">
         <v>15.05803820042827</v>
@@ -3022,10 +3022,10 @@
         <v>1.5</v>
       </c>
       <c r="AD19" t="n">
-        <v>27.29891290280062</v>
+        <v>30.12484955897654</v>
       </c>
       <c r="AE19" t="n">
-        <v>9.361719552714158</v>
+        <v>8.478713798327878</v>
       </c>
       <c r="AF19" t="n">
         <v>15.05803820042827</v>
@@ -3034,10 +3034,10 @@
         <v>1.5</v>
       </c>
       <c r="AH19" t="n">
-        <v>33.13433070710671</v>
+        <v>34.04294804829917</v>
       </c>
       <c r="AI19" t="n">
-        <v>5.107566407214144</v>
+        <v>6.261354383276984</v>
       </c>
       <c r="AJ19" t="n">
         <v>15.05803820042827</v>
@@ -3046,10 +3046,10 @@
         <v>1.5</v>
       </c>
       <c r="AL19" t="n">
-        <v>29.9312055744117</v>
+        <v>28.16446072907494</v>
       </c>
       <c r="AM19" t="n">
-        <v>8.353103299572961</v>
+        <v>8.270112832763679</v>
       </c>
       <c r="AN19" t="n">
         <v>15.05803820042827</v>
@@ -3058,10 +3058,10 @@
         <v>1.5</v>
       </c>
       <c r="AP19" t="n">
-        <v>30.05203820042827</v>
+        <v>28.90027888441666</v>
       </c>
       <c r="AQ19" t="n">
-        <v>8.291338685685453</v>
+        <v>6.575124575398896</v>
       </c>
       <c r="AR19" t="n">
         <v>15.05803820042827</v>
@@ -3084,10 +3084,10 @@
         <v>1.6</v>
       </c>
       <c r="F20" t="n">
-        <v>36.74939135865147</v>
+        <v>29.79058324051276</v>
       </c>
       <c r="G20" t="n">
-        <v>10.09474094437125</v>
+        <v>9.575607098865719</v>
       </c>
       <c r="H20" t="n">
         <v>15.06180515339463</v>
@@ -3096,10 +3096,10 @@
         <v>1.6</v>
       </c>
       <c r="J20" t="n">
-        <v>35.447039175573</v>
+        <v>30.46513481845286</v>
       </c>
       <c r="K20" t="n">
-        <v>11.67710846182061</v>
+        <v>7.882117400881855</v>
       </c>
       <c r="L20" t="n">
         <v>15.06180515339463</v>
@@ -3108,10 +3108,10 @@
         <v>1.6</v>
       </c>
       <c r="N20" t="n">
-        <v>29.9714530303794</v>
+        <v>31.78356844129504</v>
       </c>
       <c r="O20" t="n">
-        <v>11.23393798247221</v>
+        <v>8.529887610618131</v>
       </c>
       <c r="P20" t="n">
         <v>15.06180515339463</v>
@@ -3120,10 +3120,10 @@
         <v>1.6</v>
       </c>
       <c r="R20" t="n">
-        <v>30.65494000888884</v>
+        <v>31.77941630102129</v>
       </c>
       <c r="S20" t="n">
-        <v>9.163302185481523</v>
+        <v>8.054555527832475</v>
       </c>
       <c r="T20" t="n">
         <v>15.06180515339463</v>
@@ -3132,10 +3132,10 @@
         <v>1.6</v>
       </c>
       <c r="V20" t="n">
-        <v>33.01818680041167</v>
+        <v>34.3757151842333</v>
       </c>
       <c r="W20" t="n">
-        <v>8.779064490725773</v>
+        <v>10.23867109838939</v>
       </c>
       <c r="X20" t="n">
         <v>15.06180515339463</v>
@@ -3144,10 +3144,10 @@
         <v>1.6</v>
       </c>
       <c r="Z20" t="n">
-        <v>31.5505665608623</v>
+        <v>32.71243417171957</v>
       </c>
       <c r="AA20" t="n">
-        <v>8.919094442701555</v>
+        <v>12.81056985254927</v>
       </c>
       <c r="AB20" t="n">
         <v>15.06180515339463</v>
@@ -3156,10 +3156,10 @@
         <v>1.6</v>
       </c>
       <c r="AD20" t="n">
-        <v>28.45487423407196</v>
+        <v>31.90879681384252</v>
       </c>
       <c r="AE20" t="n">
-        <v>10.08730777264975</v>
+        <v>9.008078517288737</v>
       </c>
       <c r="AF20" t="n">
         <v>15.06180515339463</v>
@@ -3168,10 +3168,10 @@
         <v>1.6</v>
       </c>
       <c r="AH20" t="n">
-        <v>35.58705155044606</v>
+        <v>36.69758385634797</v>
       </c>
       <c r="AI20" t="n">
-        <v>4.887787261483064</v>
+        <v>6.297972565559868</v>
       </c>
       <c r="AJ20" t="n">
         <v>15.06180515339463</v>
@@ -3180,10 +3180,10 @@
         <v>1.6</v>
       </c>
       <c r="AL20" t="n">
-        <v>31.6855466800429</v>
+        <v>29.51276602174056</v>
       </c>
       <c r="AM20" t="n">
-        <v>8.847691839489672</v>
+        <v>8.753121781599162</v>
       </c>
       <c r="AN20" t="n">
         <v>15.06180515339463</v>
@@ -3192,10 +3192,10 @@
         <v>1.6</v>
       </c>
       <c r="AP20" t="n">
-        <v>31.81980515339464</v>
+        <v>30.41209932271378</v>
       </c>
       <c r="AQ20" t="n">
-        <v>8.779064490725773</v>
+        <v>6.681469467042205</v>
       </c>
       <c r="AR20" t="n">
         <v>15.06180515339463</v>
@@ -3218,10 +3218,10 @@
         <v>1.7</v>
       </c>
       <c r="F21" t="n">
-        <v>39.50307555266921</v>
+        <v>31.15250581090276</v>
       </c>
       <c r="G21" t="n">
-        <v>10.84560204014067</v>
+        <v>10.22264142553403</v>
       </c>
       <c r="H21" t="n">
         <v>14.967572106361</v>
@@ -3230,10 +3230,10 @@
         <v>1.7</v>
       </c>
       <c r="J21" t="n">
-        <v>37.94025293297505</v>
+        <v>31.96196770443088</v>
       </c>
       <c r="K21" t="n">
-        <v>12.7444430610799</v>
+        <v>8.190453787953393</v>
       </c>
       <c r="L21" t="n">
         <v>14.967572106361</v>
@@ -3242,10 +3242,10 @@
         <v>1.7</v>
       </c>
       <c r="N21" t="n">
-        <v>31.43116129617657</v>
+        <v>33.54576051547686</v>
       </c>
       <c r="O21" t="n">
-        <v>12.13080936947027</v>
+        <v>8.979278511026507</v>
       </c>
       <c r="P21" t="n">
         <v>14.967572106361</v>
@@ -3254,10 +3254,10 @@
         <v>1.7</v>
       </c>
       <c r="R21" t="n">
-        <v>32.18973393295406</v>
+        <v>33.53910548351298</v>
       </c>
       <c r="S21" t="n">
-        <v>9.727875529472994</v>
+        <v>8.397379540294136</v>
       </c>
       <c r="T21" t="n">
         <v>14.967572106361</v>
@@ -3266,10 +3266,10 @@
         <v>1.7</v>
       </c>
       <c r="V21" t="n">
-        <v>35.02563008278145</v>
+        <v>36.65466414336741</v>
       </c>
       <c r="W21" t="n">
-        <v>9.266790295766093</v>
+        <v>11.01831822496244</v>
       </c>
       <c r="X21" t="n">
         <v>14.967572106361</v>
@@ -3278,10 +3278,10 @@
         <v>1.7</v>
       </c>
       <c r="Z21" t="n">
-        <v>33.26448579532221</v>
+        <v>34.6175286659667</v>
       </c>
       <c r="AA21" t="n">
-        <v>9.434826238137031</v>
+        <v>13.91852725171628</v>
       </c>
       <c r="AB21" t="n">
         <v>14.967572106361</v>
@@ -3290,10 +3290,10 @@
         <v>1.7</v>
       </c>
       <c r="AD21" t="n">
-        <v>29.54965500317379</v>
+        <v>33.69436209889847</v>
       </c>
       <c r="AE21" t="n">
-        <v>10.83668223407486</v>
+        <v>9.541607127641651</v>
       </c>
       <c r="AF21" t="n">
         <v>14.967572106361</v>
@@ -3302,10 +3302,10 @@
         <v>1.7</v>
       </c>
       <c r="AH21" t="n">
-        <v>38.10826778282271</v>
+        <v>39.440906549905</v>
       </c>
       <c r="AI21" t="n">
-        <v>4.597257620674843</v>
+        <v>6.289479985567008</v>
       </c>
       <c r="AJ21" t="n">
         <v>14.967572106361</v>
@@ -3314,10 +3314,10 @@
         <v>1.7</v>
       </c>
       <c r="AL21" t="n">
-        <v>33.4398877856741</v>
+        <v>30.81912514837612</v>
       </c>
       <c r="AM21" t="n">
-        <v>9.342280379406382</v>
+        <v>9.235659044814161</v>
       </c>
       <c r="AN21" t="n">
         <v>14.967572106361</v>
@@ -3326,10 +3326,10 @@
         <v>1.7</v>
       </c>
       <c r="AP21" t="n">
-        <v>33.587572106361</v>
+        <v>31.89832510954398</v>
       </c>
       <c r="AQ21" t="n">
-        <v>9.266790295766093</v>
+        <v>6.749676267345812</v>
       </c>
       <c r="AR21" t="n">
         <v>14.967572106361</v>
@@ -3352,10 +3352,10 @@
         <v>1.8</v>
       </c>
       <c r="F22" t="n">
-        <v>42.34638858678252</v>
+        <v>32.51442838129275</v>
       </c>
       <c r="G22" t="n">
-        <v>11.62038452597636</v>
+        <v>10.86967575220234</v>
       </c>
       <c r="H22" t="n">
         <v>14.77533905932737</v>
@@ -3364,10 +3364,10 @@
         <v>1.8</v>
       </c>
       <c r="J22" t="n">
-        <v>40.49941639987124</v>
+        <v>33.43417022068268</v>
       </c>
       <c r="K22" t="n">
-        <v>13.86446936890455</v>
+        <v>8.482482046118678</v>
       </c>
       <c r="L22" t="n">
         <v>14.77533905932737</v>
@@ -3376,10 +3376,10 @@
         <v>1.8</v>
       </c>
       <c r="N22" t="n">
-        <v>32.89086956197373</v>
+        <v>35.30795258965867</v>
       </c>
       <c r="O22" t="n">
-        <v>13.02768075646834</v>
+        <v>9.428669411434884</v>
       </c>
       <c r="P22" t="n">
         <v>14.77533905932737</v>
@@ -3388,10 +3388,10 @@
         <v>1.8</v>
       </c>
       <c r="R22" t="n">
-        <v>33.70334849075552</v>
+        <v>35.29806032323426</v>
       </c>
       <c r="S22" t="n">
-        <v>10.29943501336911</v>
+        <v>8.727030662521374</v>
       </c>
       <c r="T22" t="n">
         <v>14.77533905932737</v>
@@ -3400,10 +3400,10 @@
         <v>1.8</v>
       </c>
       <c r="V22" t="n">
-        <v>37.05486212236971</v>
+        <v>38.9800841939713</v>
       </c>
       <c r="W22" t="n">
-        <v>9.754516100806413</v>
+        <v>11.824503653493</v>
       </c>
       <c r="X22" t="n">
         <v>14.77533905932737</v>
@@ -3412,10 +3412,10 @@
         <v>1.8</v>
       </c>
       <c r="Z22" t="n">
-        <v>34.97350978264516</v>
+        <v>36.52262316021383</v>
       </c>
       <c r="AA22" t="n">
-        <v>9.95310403269934</v>
+        <v>15.0264846508833</v>
       </c>
       <c r="AB22" t="n">
         <v>14.77533905932737</v>
@@ -3424,10 +3424,10 @@
         <v>1.8</v>
       </c>
       <c r="AD22" t="n">
-        <v>30.58325521010612</v>
+        <v>35.48154541414438</v>
       </c>
       <c r="AE22" t="n">
-        <v>11.60984293698951</v>
+        <v>10.07929962938662</v>
       </c>
       <c r="AF22" t="n">
         <v>14.77533905932737</v>
@@ -3436,10 +3436,10 @@
         <v>1.8</v>
       </c>
       <c r="AH22" t="n">
-        <v>40.69797940423667</v>
+        <v>42.27291612897028</v>
       </c>
       <c r="AI22" t="n">
-        <v>4.235977484789482</v>
+        <v>6.235876643298404</v>
       </c>
       <c r="AJ22" t="n">
         <v>14.77533905932737</v>
@@ -3448,10 +3448,10 @@
         <v>1.8</v>
       </c>
       <c r="AL22" t="n">
-        <v>35.19422889130529</v>
+        <v>32.0835381089816</v>
       </c>
       <c r="AM22" t="n">
-        <v>9.836868919323093</v>
+        <v>9.717724622408676</v>
       </c>
       <c r="AN22" t="n">
         <v>14.77533905932737</v>
@@ -3460,10 +3460,10 @@
         <v>1.8</v>
       </c>
       <c r="AP22" t="n">
-        <v>35.35533905932737</v>
+        <v>33.35895624490725</v>
       </c>
       <c r="AQ22" t="n">
-        <v>9.754516100806413</v>
+        <v>6.779744976309718</v>
       </c>
       <c r="AR22" t="n">
         <v>14.77533905932737</v>
@@ -3486,10 +3486,10 @@
         <v>1.9</v>
       </c>
       <c r="F23" t="n">
-        <v>45.27933046099142</v>
+        <v>33.87635095168275</v>
       </c>
       <c r="G23" t="n">
-        <v>12.41908840187834</v>
+        <v>11.51671007887065</v>
       </c>
       <c r="H23" t="n">
         <v>14.48510601229374</v>
@@ -3498,10 +3498,10 @@
         <v>1.9</v>
       </c>
       <c r="J23" t="n">
-        <v>43.12452957626159</v>
+        <v>34.88174236720827</v>
       </c>
       <c r="K23" t="n">
-        <v>15.03718738529455</v>
+        <v>8.75820217537771</v>
       </c>
       <c r="L23" t="n">
         <v>14.48510601229374</v>
@@ -3510,10 +3510,10 @@
         <v>1.9</v>
       </c>
       <c r="N23" t="n">
-        <v>34.35057782777089</v>
+        <v>37.07014466384048</v>
       </c>
       <c r="O23" t="n">
-        <v>13.9245521434664</v>
+        <v>9.87806031184326</v>
       </c>
       <c r="P23" t="n">
         <v>14.48510601229374</v>
@@ -3522,10 +3522,10 @@
         <v>1.9</v>
       </c>
       <c r="R23" t="n">
-        <v>35.19578368229325</v>
+        <v>37.05628082018511</v>
       </c>
       <c r="S23" t="n">
-        <v>10.87798063716989</v>
+        <v>9.043508894514188</v>
       </c>
       <c r="T23" t="n">
         <v>14.48510601229374</v>
@@ -3534,10 +3534,10 @@
         <v>1.9</v>
       </c>
       <c r="V23" t="n">
-        <v>39.10588291917647</v>
+        <v>41.35197533604499</v>
       </c>
       <c r="W23" t="n">
-        <v>10.24224190584673</v>
+        <v>12.65722738398109</v>
       </c>
       <c r="X23" t="n">
         <v>14.48510601229374</v>
@@ -3546,10 +3546,10 @@
         <v>1.9</v>
       </c>
       <c r="Z23" t="n">
-        <v>36.67763852283116</v>
+        <v>38.42771765446096</v>
       </c>
       <c r="AA23" t="n">
-        <v>10.47392782638848</v>
+        <v>16.13444205005031</v>
       </c>
       <c r="AB23" t="n">
         <v>14.48510601229374</v>
@@ -3558,10 +3558,10 @@
         <v>1.9</v>
       </c>
       <c r="AD23" t="n">
-        <v>31.55567485486895</v>
+        <v>37.27034675958025</v>
       </c>
       <c r="AE23" t="n">
-        <v>12.40678988139368</v>
+        <v>10.62115602252364</v>
       </c>
       <c r="AF23" t="n">
         <v>14.48510601229374</v>
@@ -3570,10 +3570,10 @@
         <v>1.9</v>
       </c>
       <c r="AH23" t="n">
-        <v>43.35618641468792</v>
+        <v>45.1936125935438</v>
       </c>
       <c r="AI23" t="n">
-        <v>3.80394685382698</v>
+        <v>6.137162538754056</v>
       </c>
       <c r="AJ23" t="n">
         <v>14.48510601229374</v>
@@ -3582,10 +3582,10 @@
         <v>1.9</v>
       </c>
       <c r="AL23" t="n">
-        <v>36.94856999693649</v>
+        <v>33.306004903557</v>
       </c>
       <c r="AM23" t="n">
-        <v>10.3314574592398</v>
+        <v>10.19931851438271</v>
       </c>
       <c r="AN23" t="n">
         <v>14.48510601229374</v>
@@ -3594,10 +3594,10 @@
         <v>1.9</v>
       </c>
       <c r="AP23" t="n">
-        <v>37.12310601229374</v>
+        <v>34.7939927288036</v>
       </c>
       <c r="AQ23" t="n">
-        <v>10.24224190584673</v>
+        <v>6.771675593933922</v>
       </c>
       <c r="AR23" t="n">
         <v>14.48510601229374</v>
@@ -3620,10 +3620,10 @@
         <v>2</v>
       </c>
       <c r="F24" t="n">
-        <v>48.30190117529589</v>
+        <v>35.23827352207274</v>
       </c>
       <c r="G24" t="n">
-        <v>13.24171366784661</v>
+        <v>12.16374440553896</v>
       </c>
       <c r="H24" t="n">
         <v>14.09687296526011</v>
@@ -3632,10 +3632,10 @@
         <v>2</v>
       </c>
       <c r="J24" t="n">
-        <v>45.81559246214609</v>
+        <v>36.30468414400764</v>
       </c>
       <c r="K24" t="n">
-        <v>16.26259711024992</v>
+        <v>9.017614175730488</v>
       </c>
       <c r="L24" t="n">
         <v>14.09687296526011</v>
@@ -3644,10 +3644,10 @@
         <v>2</v>
       </c>
       <c r="N24" t="n">
-        <v>35.81028609356805</v>
+        <v>38.83233673802229</v>
       </c>
       <c r="O24" t="n">
-        <v>14.82142353046446</v>
+        <v>10.32745121225164</v>
       </c>
       <c r="P24" t="n">
         <v>14.09687296526011</v>
@@ -3656,10 +3656,10 @@
         <v>2</v>
       </c>
       <c r="R24" t="n">
-        <v>36.66703950756724</v>
+        <v>38.81376697436554</v>
       </c>
       <c r="S24" t="n">
-        <v>11.46351240087531</v>
+        <v>9.346814236272579</v>
       </c>
       <c r="T24" t="n">
         <v>14.09687296526011</v>
@@ -3668,10 +3668,10 @@
         <v>2</v>
       </c>
       <c r="V24" t="n">
-        <v>41.17869247320172</v>
+        <v>43.77033756958848</v>
       </c>
       <c r="W24" t="n">
-        <v>10.72996771088705</v>
+        <v>13.51648941642669</v>
       </c>
       <c r="X24" t="n">
         <v>14.09687296526011</v>
@@ -3680,10 +3680,10 @@
         <v>2</v>
       </c>
       <c r="Z24" t="n">
-        <v>38.37687201588021</v>
+        <v>40.33281214870809</v>
       </c>
       <c r="AA24" t="n">
-        <v>10.99729761920445</v>
+        <v>17.24239944921732</v>
       </c>
       <c r="AB24" t="n">
         <v>14.09687296526011</v>
@@ -3692,10 +3692,10 @@
         <v>2</v>
       </c>
       <c r="AD24" t="n">
-        <v>32.46691393746227</v>
+        <v>39.06076613520608</v>
       </c>
       <c r="AE24" t="n">
-        <v>13.22752306728737</v>
+        <v>11.16717630705271</v>
       </c>
       <c r="AF24" t="n">
         <v>14.09687296526011</v>
@@ -3704,10 +3704,10 @@
         <v>2</v>
       </c>
       <c r="AH24" t="n">
-        <v>46.08288881417647</v>
+        <v>48.20299594362556</v>
       </c>
       <c r="AI24" t="n">
-        <v>3.301165727787339</v>
+        <v>5.993337671933965</v>
       </c>
       <c r="AJ24" t="n">
         <v>14.09687296526011</v>
@@ -3716,10 +3716,10 @@
         <v>2</v>
       </c>
       <c r="AL24" t="n">
-        <v>38.70291110256769</v>
+        <v>34.48652553210233</v>
       </c>
       <c r="AM24" t="n">
-        <v>10.82604599915651</v>
+        <v>10.68044072073625</v>
       </c>
       <c r="AN24" t="n">
         <v>14.09687296526011</v>
@@ -3728,10 +3728,10 @@
         <v>2</v>
       </c>
       <c r="AP24" t="n">
-        <v>38.89087296526011</v>
+        <v>36.20343456123302</v>
       </c>
       <c r="AQ24" t="n">
-        <v>10.72996771088705</v>
+        <v>6.725468120218425</v>
       </c>
       <c r="AR24" t="n">
         <v>14.09687296526011</v>
@@ -3754,10 +3754,10 @@
         <v>2.1</v>
       </c>
       <c r="F25" t="n">
-        <v>51.41410072969594</v>
+        <v>36.60019609246273</v>
       </c>
       <c r="G25" t="n">
-        <v>14.08826032388115</v>
+        <v>12.81077873220727</v>
       </c>
       <c r="H25" t="n">
         <v>13.61063991822647</v>
@@ -3766,10 +3766,10 @@
         <v>2.1</v>
       </c>
       <c r="J25" t="n">
-        <v>48.57260505752475</v>
+        <v>37.7029955510808</v>
       </c>
       <c r="K25" t="n">
-        <v>17.54069854377065</v>
+        <v>9.260718047177013</v>
       </c>
       <c r="L25" t="n">
         <v>13.61063991822647</v>
@@ -3778,10 +3778,10 @@
         <v>2.1</v>
       </c>
       <c r="N25" t="n">
-        <v>37.26999435936521</v>
+        <v>40.5945288122041</v>
       </c>
       <c r="O25" t="n">
-        <v>15.71829491746252</v>
+        <v>10.77684211266001</v>
       </c>
       <c r="P25" t="n">
         <v>13.61063991822647</v>
@@ -3790,10 +3790,10 @@
         <v>2.1</v>
       </c>
       <c r="R25" t="n">
-        <v>38.11711596657748</v>
+        <v>40.57051878577553</v>
       </c>
       <c r="S25" t="n">
-        <v>12.05603030448538</v>
+        <v>9.636946687796545</v>
       </c>
       <c r="T25" t="n">
         <v>13.61063991822647</v>
@@ -3802,10 +3802,10 @@
         <v>2.1</v>
       </c>
       <c r="V25" t="n">
-        <v>43.27329078444546</v>
+        <v>46.23517089460176</v>
       </c>
       <c r="W25" t="n">
-        <v>11.21769351592737</v>
+        <v>14.40228975082982</v>
       </c>
       <c r="X25" t="n">
         <v>13.61063991822647</v>
@@ -3814,10 +3814,10 @@
         <v>2.1</v>
       </c>
       <c r="Z25" t="n">
-        <v>40.0712102617923</v>
+        <v>42.23790664295522</v>
       </c>
       <c r="AA25" t="n">
-        <v>11.52321341114726</v>
+        <v>18.35035684838434</v>
       </c>
       <c r="AB25" t="n">
         <v>13.61063991822647</v>
@@ -3826,10 +3826,10 @@
         <v>2.1</v>
       </c>
       <c r="AD25" t="n">
-        <v>33.3169724578861</v>
+        <v>40.85280354102187</v>
       </c>
       <c r="AE25" t="n">
-        <v>14.0720424946706</v>
+        <v>11.71736048297384</v>
       </c>
       <c r="AF25" t="n">
         <v>13.61063991822647</v>
@@ -3838,10 +3838,10 @@
         <v>2.1</v>
       </c>
       <c r="AH25" t="n">
-        <v>48.87808660270232</v>
+        <v>51.30106617921557</v>
       </c>
       <c r="AI25" t="n">
-        <v>2.727634106670557</v>
+        <v>5.80440204283813</v>
       </c>
       <c r="AJ25" t="n">
         <v>13.61063991822647</v>
@@ -3850,10 +3850,10 @@
         <v>2.1</v>
       </c>
       <c r="AL25" t="n">
-        <v>40.45725220819889</v>
+        <v>35.62509999461759</v>
       </c>
       <c r="AM25" t="n">
-        <v>11.32063453907323</v>
+        <v>11.16109124146932</v>
       </c>
       <c r="AN25" t="n">
         <v>13.61063991822647</v>
@@ -3862,10 +3862,10 @@
         <v>2.1</v>
       </c>
       <c r="AP25" t="n">
-        <v>40.65863991822648</v>
+        <v>37.58728174219552</v>
       </c>
       <c r="AQ25" t="n">
-        <v>11.21769351592737</v>
+        <v>6.641122555163227</v>
       </c>
       <c r="AR25" t="n">
         <v>13.61063991822647</v>
@@ -3888,10 +3888,10 @@
         <v>2.2</v>
       </c>
       <c r="F26" t="n">
-        <v>54.61592912419157</v>
+        <v>37.96211866285272</v>
       </c>
       <c r="G26" t="n">
-        <v>14.95872836998197</v>
+        <v>13.45781305887558</v>
       </c>
       <c r="H26" t="n">
         <v>13.02640687119284</v>
@@ -3900,10 +3900,10 @@
         <v>2.2</v>
       </c>
       <c r="J26" t="n">
-        <v>51.39556736239755</v>
+        <v>39.07667658842774</v>
       </c>
       <c r="K26" t="n">
-        <v>18.87149168585674</v>
+        <v>9.487513789717285</v>
       </c>
       <c r="L26" t="n">
         <v>13.02640687119284</v>
@@ -3912,10 +3912,10 @@
         <v>2.2</v>
       </c>
       <c r="N26" t="n">
-        <v>38.72970262516237</v>
+        <v>42.35672088638592</v>
       </c>
       <c r="O26" t="n">
-        <v>16.61516630446058</v>
+        <v>11.22623301306839</v>
       </c>
       <c r="P26" t="n">
         <v>13.02640687119284</v>
@@ -3924,10 +3924,10 @@
         <v>2.2</v>
       </c>
       <c r="R26" t="n">
-        <v>39.54601305932398</v>
+        <v>42.32653625441511</v>
       </c>
       <c r="S26" t="n">
-        <v>12.6555343480001</v>
+        <v>9.913906249086088</v>
       </c>
       <c r="T26" t="n">
         <v>13.02640687119284</v>
@@ -3936,10 +3936,10 @@
         <v>2.2</v>
       </c>
       <c r="V26" t="n">
-        <v>45.3896778529077</v>
+        <v>48.74647531108484</v>
       </c>
       <c r="W26" t="n">
-        <v>11.70541932096769</v>
+        <v>15.31462838719047</v>
       </c>
       <c r="X26" t="n">
         <v>13.02640687119284</v>
@@ -3948,10 +3948,10 @@
         <v>2.2</v>
       </c>
       <c r="Z26" t="n">
-        <v>41.76065326056744</v>
+        <v>44.14300113720235</v>
       </c>
       <c r="AA26" t="n">
-        <v>12.0516752022169</v>
+        <v>19.45831424755135</v>
       </c>
       <c r="AB26" t="n">
         <v>13.02640687119284</v>
@@ -3960,10 +3960,10 @@
         <v>2.2</v>
       </c>
       <c r="AD26" t="n">
-        <v>34.10585041614041</v>
+        <v>42.64645897702763</v>
       </c>
       <c r="AE26" t="n">
-        <v>14.94034816354335</v>
+        <v>12.27170855028703</v>
       </c>
       <c r="AF26" t="n">
         <v>13.02640687119284</v>
@@ -3972,10 +3972,10 @@
         <v>2.2</v>
       </c>
       <c r="AH26" t="n">
-        <v>51.74177978026546</v>
+        <v>54.48782330031381</v>
       </c>
       <c r="AI26" t="n">
-        <v>2.083351990476635</v>
+        <v>5.570355651466551</v>
       </c>
       <c r="AJ26" t="n">
         <v>13.02640687119284</v>
@@ -3984,10 +3984,10 @@
         <v>2.2</v>
       </c>
       <c r="AL26" t="n">
-        <v>42.21159331383009</v>
+        <v>36.72172829110278</v>
       </c>
       <c r="AM26" t="n">
-        <v>11.81522307898994</v>
+        <v>11.6412700765819</v>
       </c>
       <c r="AN26" t="n">
         <v>13.02640687119284</v>
@@ -3996,10 +3996,10 @@
         <v>2.2</v>
       </c>
       <c r="AP26" t="n">
-        <v>42.42640687119285</v>
+        <v>38.94553427169109</v>
       </c>
       <c r="AQ26" t="n">
-        <v>11.70541932096769</v>
+        <v>6.518638898768327</v>
       </c>
       <c r="AR26" t="n">
         <v>13.02640687119284</v>
@@ -4022,10 +4022,10 @@
         <v>2.3</v>
       </c>
       <c r="F27" t="n">
-        <v>57.90738635878277</v>
+        <v>39.32404123324272</v>
       </c>
       <c r="G27" t="n">
-        <v>15.85311780614908</v>
+        <v>14.10484738554389</v>
       </c>
       <c r="H27" t="n">
         <v>12.34417382415921</v>
@@ -4034,10 +4034,10 @@
         <v>2.3</v>
       </c>
       <c r="J27" t="n">
-        <v>54.28447937676451</v>
+        <v>40.42572725604848</v>
       </c>
       <c r="K27" t="n">
-        <v>20.2549765365082</v>
+        <v>9.698001403351304</v>
       </c>
       <c r="L27" t="n">
         <v>12.34417382415921</v>
@@ -4046,10 +4046,10 @@
         <v>2.3</v>
       </c>
       <c r="N27" t="n">
-        <v>40.18941089095954</v>
+        <v>44.11891296056773</v>
       </c>
       <c r="O27" t="n">
-        <v>17.51203769145864</v>
+        <v>11.67562391347677</v>
       </c>
       <c r="P27" t="n">
         <v>12.34417382415921</v>
@@ -4058,10 +4058,10 @@
         <v>2.3</v>
       </c>
       <c r="R27" t="n">
-        <v>40.95373078580674</v>
+        <v>44.08181938028426</v>
       </c>
       <c r="S27" t="n">
-        <v>13.26202453141947</v>
+        <v>10.17769292014121</v>
       </c>
       <c r="T27" t="n">
         <v>12.34417382415921</v>
@@ -4070,10 +4070,10 @@
         <v>2.3</v>
       </c>
       <c r="V27" t="n">
-        <v>47.52785367858843</v>
+        <v>51.3042508190377</v>
       </c>
       <c r="W27" t="n">
-        <v>12.19314512600801</v>
+        <v>16.25350532550863</v>
       </c>
       <c r="X27" t="n">
         <v>12.34417382415921</v>
@@ -4082,10 +4082,10 @@
         <v>2.3</v>
       </c>
       <c r="Z27" t="n">
-        <v>43.44520101220564</v>
+        <v>46.04809563144948</v>
       </c>
       <c r="AA27" t="n">
-        <v>12.58268299241337</v>
+        <v>20.56627164671836</v>
       </c>
       <c r="AB27" t="n">
         <v>12.34417382415921</v>
@@ -4094,10 +4094,10 @@
         <v>2.3</v>
       </c>
       <c r="AD27" t="n">
-        <v>34.83354781222523</v>
+        <v>44.44173244322334</v>
       </c>
       <c r="AE27" t="n">
-        <v>15.83244007390562</v>
+        <v>12.83022050899226</v>
       </c>
       <c r="AF27" t="n">
         <v>12.34417382415921</v>
@@ -4106,10 +4106,10 @@
         <v>2.3</v>
       </c>
       <c r="AH27" t="n">
-        <v>54.67396834686591</v>
+        <v>57.76326730692031</v>
       </c>
       <c r="AI27" t="n">
-        <v>1.368319379205573</v>
+        <v>5.291198497819228</v>
       </c>
       <c r="AJ27" t="n">
         <v>12.34417382415921</v>
@@ -4118,10 +4118,10 @@
         <v>2.3</v>
       </c>
       <c r="AL27" t="n">
-        <v>43.96593441946128</v>
+        <v>37.77641042155789</v>
       </c>
       <c r="AM27" t="n">
-        <v>12.30981161890665</v>
+        <v>12.12097722607399</v>
       </c>
       <c r="AN27" t="n">
         <v>12.34417382415921</v>
@@ -4130,10 +4130,10 @@
         <v>2.3</v>
       </c>
       <c r="AP27" t="n">
-        <v>44.19417382415921</v>
+        <v>40.27819214971974</v>
       </c>
       <c r="AQ27" t="n">
-        <v>12.19314512600801</v>
+        <v>6.358017151033727</v>
       </c>
       <c r="AR27" t="n">
         <v>12.34417382415921</v>
@@ -4156,10 +4156,10 @@
         <v>2.4</v>
       </c>
       <c r="F28" t="n">
-        <v>61.28847243346956</v>
+        <v>40.68596380363271</v>
       </c>
       <c r="G28" t="n">
-        <v>16.77142863238246</v>
+        <v>14.7518817122122</v>
       </c>
       <c r="H28" t="n">
         <v>11.56394077712558</v>
@@ -4168,10 +4168,10 @@
         <v>2.4</v>
       </c>
       <c r="J28" t="n">
-        <v>57.23934110062562</v>
+        <v>41.75014755394299</v>
       </c>
       <c r="K28" t="n">
-        <v>21.69115309572501</v>
+        <v>9.89218088807907</v>
       </c>
       <c r="L28" t="n">
         <v>11.56394077712558</v>
@@ -4180,10 +4180,10 @@
         <v>2.4</v>
       </c>
       <c r="N28" t="n">
-        <v>41.6491191567567</v>
+        <v>45.88110503474954</v>
       </c>
       <c r="O28" t="n">
-        <v>18.4089090784567</v>
+        <v>12.12501481388514</v>
       </c>
       <c r="P28" t="n">
         <v>11.56394077712558</v>
@@ -4192,10 +4192,10 @@
         <v>2.4</v>
       </c>
       <c r="R28" t="n">
-        <v>42.34026914602576</v>
+        <v>45.83636816338299</v>
       </c>
       <c r="S28" t="n">
-        <v>13.87550085474349</v>
+        <v>10.4283067009619</v>
       </c>
       <c r="T28" t="n">
         <v>11.56394077712558</v>
@@ -4204,10 +4204,10 @@
         <v>2.4</v>
       </c>
       <c r="V28" t="n">
-        <v>49.68781826148765</v>
+        <v>53.90849741846037</v>
       </c>
       <c r="W28" t="n">
-        <v>12.68087093104833</v>
+        <v>17.21892056578432</v>
       </c>
       <c r="X28" t="n">
         <v>11.56394077712558</v>
@@ -4216,10 +4216,10 @@
         <v>2.4</v>
       </c>
       <c r="Z28" t="n">
-        <v>45.12485351670688</v>
+        <v>47.95319012569662</v>
       </c>
       <c r="AA28" t="n">
-        <v>13.11623678173667</v>
+        <v>21.67422904588538</v>
       </c>
       <c r="AB28" t="n">
         <v>11.56394077712558</v>
@@ -4228,10 +4228,10 @@
         <v>2.4</v>
       </c>
       <c r="AD28" t="n">
-        <v>35.50006464614054</v>
+        <v>46.23862393960902</v>
       </c>
       <c r="AE28" t="n">
-        <v>16.74831822575743</v>
+        <v>13.39289635908955</v>
       </c>
       <c r="AF28" t="n">
         <v>11.56394077712558</v>
@@ -4240,10 +4240,10 @@
         <v>2.4</v>
       </c>
       <c r="AH28" t="n">
-        <v>57.67465230250365</v>
+        <v>61.12739819903504</v>
       </c>
       <c r="AI28" t="n">
-        <v>0.5825362728573711</v>
+        <v>4.966930581896162</v>
       </c>
       <c r="AJ28" t="n">
         <v>11.56394077712558</v>
@@ -4252,10 +4252,10 @@
         <v>2.4</v>
       </c>
       <c r="AL28" t="n">
-        <v>45.72027552509248</v>
+        <v>38.78914638598292</v>
       </c>
       <c r="AM28" t="n">
-        <v>12.80440015882336</v>
+        <v>12.6002126899456</v>
       </c>
       <c r="AN28" t="n">
         <v>11.56394077712558</v>
@@ -4264,10 +4264,10 @@
         <v>2.4</v>
       </c>
       <c r="AP28" t="n">
-        <v>45.96194077712558</v>
+        <v>41.58525537628147</v>
       </c>
       <c r="AQ28" t="n">
-        <v>12.68087093104833</v>
+        <v>6.159257311959426</v>
       </c>
       <c r="AR28" t="n">
         <v>11.56394077712558</v>
@@ -4290,10 +4290,10 @@
         <v>2.5</v>
       </c>
       <c r="F29" t="n">
-        <v>64.75918734825193</v>
+        <v>42.0478863740227</v>
       </c>
       <c r="G29" t="n">
-        <v>17.71366084868213</v>
+        <v>15.39891603888051</v>
       </c>
       <c r="H29" t="n">
         <v>10.68570773009194</v>
@@ -4302,10 +4302,10 @@
         <v>2.5</v>
       </c>
       <c r="J29" t="n">
-        <v>60.26015253398088</v>
+        <v>43.0499374821113</v>
       </c>
       <c r="K29" t="n">
-        <v>23.18002136350718</v>
+        <v>10.07005224390058</v>
       </c>
       <c r="L29" t="n">
         <v>10.68570773009194</v>
@@ -4314,10 +4314,10 @@
         <v>2.5</v>
       </c>
       <c r="N29" t="n">
-        <v>43.10882742255386</v>
+        <v>47.64329710893135</v>
       </c>
       <c r="O29" t="n">
-        <v>19.30578046545476</v>
+        <v>12.57440571429352</v>
       </c>
       <c r="P29" t="n">
         <v>10.68570773009194</v>
@@ -4326,10 +4326,10 @@
         <v>2.5</v>
       </c>
       <c r="R29" t="n">
-        <v>43.70562813998104</v>
+        <v>47.59018260371128</v>
       </c>
       <c r="S29" t="n">
-        <v>14.49596331797216</v>
+        <v>10.66574759154818</v>
       </c>
       <c r="T29" t="n">
         <v>10.68570773009194</v>
@@ -4338,10 +4338,10 @@
         <v>2.5</v>
       </c>
       <c r="V29" t="n">
-        <v>51.84778284438687</v>
+        <v>56.55921510935283</v>
       </c>
       <c r="W29" t="n">
-        <v>13.16859673608865</v>
+        <v>18.21087410801753</v>
       </c>
       <c r="X29" t="n">
         <v>10.68570773009194</v>
@@ -4350,10 +4350,10 @@
         <v>2.5</v>
       </c>
       <c r="Z29" t="n">
-        <v>46.79961077407117</v>
+        <v>49.85828461994375</v>
       </c>
       <c r="AA29" t="n">
-        <v>13.65233657018681</v>
+        <v>22.78218644505239</v>
       </c>
       <c r="AB29" t="n">
         <v>10.68570773009194</v>
@@ -4362,10 +4362,10 @@
         <v>2.5</v>
       </c>
       <c r="AD29" t="n">
-        <v>36.10540091788634</v>
+        <v>48.03713346618466</v>
       </c>
       <c r="AE29" t="n">
-        <v>17.68798261909876</v>
+        <v>13.9597361005789</v>
       </c>
       <c r="AF29" t="n">
         <v>10.68570773009194</v>
@@ -4374,10 +4374,10 @@
         <v>2.5</v>
       </c>
       <c r="AH29" t="n">
-        <v>60.74383164717869</v>
+        <v>64.58021597665801</v>
       </c>
       <c r="AI29" t="n">
-        <v>-0.2739973285679713</v>
+        <v>4.597551903697352</v>
       </c>
       <c r="AJ29" t="n">
         <v>10.68570773009194</v>
@@ -4386,10 +4386,10 @@
         <v>2.5</v>
       </c>
       <c r="AL29" t="n">
-        <v>47.47461663072368</v>
+        <v>39.75993618437789</v>
       </c>
       <c r="AM29" t="n">
-        <v>13.29898869874007</v>
+        <v>13.07897646819673</v>
       </c>
       <c r="AN29" t="n">
         <v>10.68570773009194</v>
@@ -4398,10 +4398,10 @@
         <v>2.5</v>
       </c>
       <c r="AP29" t="n">
-        <v>47.72970773009195</v>
+        <v>42.86672395137627</v>
       </c>
       <c r="AQ29" t="n">
-        <v>13.16859673608865</v>
+        <v>5.922359381545423</v>
       </c>
       <c r="AR29" t="n">
         <v>10.68570773009194</v>
@@ -4424,10 +4424,10 @@
         <v>2.6</v>
       </c>
       <c r="F30" t="n">
-        <v>68.22990226303429</v>
+        <v>43.4098089444127</v>
       </c>
       <c r="G30" t="n">
-        <v>18.6558930649818</v>
+        <v>16.04595036554882</v>
       </c>
       <c r="H30" t="n">
         <v>9.709474683058312</v>
@@ -4436,10 +4436,10 @@
         <v>2.6</v>
       </c>
       <c r="J30" t="n">
-        <v>63.28096396733614</v>
+        <v>44.3497274102796</v>
       </c>
       <c r="K30" t="n">
-        <v>24.66888963128935</v>
+        <v>10.24792359972209</v>
       </c>
       <c r="L30" t="n">
         <v>9.709474683058312</v>
@@ -4448,10 +4448,10 @@
         <v>2.6</v>
       </c>
       <c r="N30" t="n">
-        <v>44.56853568835102</v>
+        <v>49.40548918311316</v>
       </c>
       <c r="O30" t="n">
-        <v>20.20265185245282</v>
+        <v>13.0237966147019</v>
       </c>
       <c r="P30" t="n">
         <v>9.709474683058312</v>
@@ -4460,10 +4460,10 @@
         <v>2.6</v>
       </c>
       <c r="R30" t="n">
-        <v>45.07098713393631</v>
+        <v>49.34399704403958</v>
       </c>
       <c r="S30" t="n">
-        <v>15.11642578120083</v>
+        <v>10.90318848213445</v>
       </c>
       <c r="T30" t="n">
         <v>9.709474683058312</v>
@@ -4472,10 +4472,10 @@
         <v>2.6</v>
       </c>
       <c r="V30" t="n">
-        <v>54.00774742728609</v>
+        <v>59.20993280024528</v>
       </c>
       <c r="W30" t="n">
-        <v>13.65632254112897</v>
+        <v>19.20282765025074</v>
       </c>
       <c r="X30" t="n">
         <v>9.709474683058312</v>
@@ -4484,10 +4484,10 @@
         <v>2.6</v>
       </c>
       <c r="Z30" t="n">
-        <v>48.47436803143546</v>
+        <v>51.76337911419088</v>
       </c>
       <c r="AA30" t="n">
-        <v>14.18843635863694</v>
+        <v>23.8901438442194</v>
       </c>
       <c r="AB30" t="n">
         <v>9.709474683058312</v>
@@ -4496,10 +4496,10 @@
         <v>2.6</v>
       </c>
       <c r="AD30" t="n">
-        <v>36.71073718963215</v>
+        <v>49.83564299276029</v>
       </c>
       <c r="AE30" t="n">
-        <v>18.62764701244009</v>
+        <v>14.52657584206824</v>
       </c>
       <c r="AF30" t="n">
         <v>9.709474683058312</v>
@@ -4508,10 +4508,10 @@
         <v>2.6</v>
       </c>
       <c r="AH30" t="n">
-        <v>63.81301099185373</v>
+        <v>68.03303375428098</v>
       </c>
       <c r="AI30" t="n">
-        <v>-1.130530929993314</v>
+        <v>4.228173225498542</v>
       </c>
       <c r="AJ30" t="n">
         <v>9.709474683058312</v>
@@ -4520,10 +4520,10 @@
         <v>2.6</v>
       </c>
       <c r="AL30" t="n">
-        <v>49.22895773635488</v>
+        <v>40.73072598277285</v>
       </c>
       <c r="AM30" t="n">
-        <v>13.79357723865678</v>
+        <v>13.55774024644786</v>
       </c>
       <c r="AN30" t="n">
         <v>9.709474683058312</v>
@@ -4532,10 +4532,10 @@
         <v>2.6</v>
       </c>
       <c r="AP30" t="n">
-        <v>49.49747468305832</v>
+        <v>44.14819252647108</v>
       </c>
       <c r="AQ30" t="n">
-        <v>13.65632254112897</v>
+        <v>5.68546145113142</v>
       </c>
       <c r="AR30" t="n">
         <v>9.709474683058312</v>
@@ -4558,10 +4558,10 @@
         <v>2.7</v>
       </c>
       <c r="F31" t="n">
-        <v>71.70061717781665</v>
+        <v>44.77173151480269</v>
       </c>
       <c r="G31" t="n">
-        <v>19.59812528128147</v>
+        <v>16.69298469221713</v>
       </c>
       <c r="H31" t="n">
         <v>8.635241636024681</v>
@@ -4570,10 +4570,10 @@
         <v>2.7</v>
       </c>
       <c r="J31" t="n">
-        <v>66.3017754006914</v>
+        <v>45.6495173384479</v>
       </c>
       <c r="K31" t="n">
-        <v>26.15775789907153</v>
+        <v>10.42579495554361</v>
       </c>
       <c r="L31" t="n">
         <v>8.635241636024681</v>
@@ -4582,10 +4582,10 @@
         <v>2.7</v>
       </c>
       <c r="N31" t="n">
-        <v>46.02824395414818</v>
+        <v>51.16768125729497</v>
       </c>
       <c r="O31" t="n">
-        <v>21.09952323945089</v>
+        <v>13.47318751511027</v>
       </c>
       <c r="P31" t="n">
         <v>8.635241636024681</v>
@@ -4594,10 +4594,10 @@
         <v>2.7</v>
       </c>
       <c r="R31" t="n">
-        <v>46.43634612789159</v>
+        <v>51.09781148436788</v>
       </c>
       <c r="S31" t="n">
-        <v>15.7368882444295</v>
+        <v>11.14062937272072</v>
       </c>
       <c r="T31" t="n">
         <v>8.635241636024681</v>
@@ -4606,10 +4606,10 @@
         <v>2.7</v>
       </c>
       <c r="V31" t="n">
-        <v>56.16771201018531</v>
+        <v>61.86065049113774</v>
       </c>
       <c r="W31" t="n">
-        <v>14.14404834616929</v>
+        <v>20.19478119248394</v>
       </c>
       <c r="X31" t="n">
         <v>8.635241636024681</v>
@@ -4618,10 +4618,10 @@
         <v>2.7</v>
       </c>
       <c r="Z31" t="n">
-        <v>50.14912528879975</v>
+        <v>53.66847360843801</v>
       </c>
       <c r="AA31" t="n">
-        <v>14.72453614708708</v>
+        <v>24.99810124338642</v>
       </c>
       <c r="AB31" t="n">
         <v>8.635241636024681</v>
@@ -4630,10 +4630,10 @@
         <v>2.7</v>
       </c>
       <c r="AD31" t="n">
-        <v>37.31607346137795</v>
+        <v>51.63415251933593</v>
       </c>
       <c r="AE31" t="n">
-        <v>19.56731140578142</v>
+        <v>15.09341558355759</v>
       </c>
       <c r="AF31" t="n">
         <v>8.635241636024681</v>
@@ -4642,10 +4642,10 @@
         <v>2.7</v>
       </c>
       <c r="AH31" t="n">
-        <v>66.88219033652877</v>
+        <v>71.48585153190395</v>
       </c>
       <c r="AI31" t="n">
-        <v>-1.987064531418656</v>
+        <v>3.858794547299731</v>
       </c>
       <c r="AJ31" t="n">
         <v>8.635241636024681</v>
@@ -4654,10 +4654,10 @@
         <v>2.7</v>
       </c>
       <c r="AL31" t="n">
-        <v>50.98329884198608</v>
+        <v>41.70151578116781</v>
       </c>
       <c r="AM31" t="n">
-        <v>14.28816577857349</v>
+        <v>14.03650402469899</v>
       </c>
       <c r="AN31" t="n">
         <v>8.635241636024681</v>
@@ -4666,10 +4666,10 @@
         <v>2.7</v>
       </c>
       <c r="AP31" t="n">
-        <v>51.26524163602469</v>
+        <v>45.42966110156588</v>
       </c>
       <c r="AQ31" t="n">
-        <v>14.14404834616929</v>
+        <v>5.448563520717418</v>
       </c>
       <c r="AR31" t="n">
         <v>8.635241636024681</v>
@@ -4692,10 +4692,10 @@
         <v>2.8</v>
       </c>
       <c r="F32" t="n">
-        <v>75.17133209259902</v>
+        <v>46.13365408519268</v>
       </c>
       <c r="G32" t="n">
-        <v>20.54035749758114</v>
+        <v>17.34001901888544</v>
       </c>
       <c r="H32" t="n">
         <v>7.463008588991048</v>
@@ -4704,10 +4704,10 @@
         <v>2.8</v>
       </c>
       <c r="J32" t="n">
-        <v>69.32258683404666</v>
+        <v>46.9493072666162</v>
       </c>
       <c r="K32" t="n">
-        <v>27.6466261668537</v>
+        <v>10.60366631136512</v>
       </c>
       <c r="L32" t="n">
         <v>7.463008588991048</v>
@@ -4716,10 +4716,10 @@
         <v>2.8</v>
       </c>
       <c r="N32" t="n">
-        <v>47.48795221994534</v>
+        <v>52.92987333147678</v>
       </c>
       <c r="O32" t="n">
-        <v>21.99639462644895</v>
+        <v>13.92257841551865</v>
       </c>
       <c r="P32" t="n">
         <v>7.463008588991048</v>
@@ -4728,10 +4728,10 @@
         <v>2.8</v>
       </c>
       <c r="R32" t="n">
-        <v>47.80170512184687</v>
+        <v>52.85162592469618</v>
       </c>
       <c r="S32" t="n">
-        <v>16.35735070765817</v>
+        <v>11.378070263307</v>
       </c>
       <c r="T32" t="n">
         <v>7.463008588991048</v>
@@ -4740,10 +4740,10 @@
         <v>2.8</v>
       </c>
       <c r="V32" t="n">
-        <v>58.32767659308453</v>
+        <v>64.5113681820302</v>
       </c>
       <c r="W32" t="n">
-        <v>14.63177415120961</v>
+        <v>21.18673473471715</v>
       </c>
       <c r="X32" t="n">
         <v>7.463008588991048</v>
@@ -4752,10 +4752,10 @@
         <v>2.8</v>
       </c>
       <c r="Z32" t="n">
-        <v>51.82388254616404</v>
+        <v>55.57356810268514</v>
       </c>
       <c r="AA32" t="n">
-        <v>15.26063593553721</v>
+        <v>26.10605864255343</v>
       </c>
       <c r="AB32" t="n">
         <v>7.463008588991048</v>
@@ -4764,10 +4764,10 @@
         <v>2.8</v>
       </c>
       <c r="AD32" t="n">
-        <v>37.92140973312376</v>
+        <v>53.43266204591156</v>
       </c>
       <c r="AE32" t="n">
-        <v>20.50697579912275</v>
+        <v>15.66025532504693</v>
       </c>
       <c r="AF32" t="n">
         <v>7.463008588991048</v>
@@ -4776,10 +4776,10 @@
         <v>2.8</v>
       </c>
       <c r="AH32" t="n">
-        <v>69.9513696812038</v>
+        <v>74.93866930952692</v>
       </c>
       <c r="AI32" t="n">
-        <v>-2.843598132843999</v>
+        <v>3.489415869100921</v>
       </c>
       <c r="AJ32" t="n">
         <v>7.463008588991048</v>
@@ -4788,10 +4788,10 @@
         <v>2.8</v>
       </c>
       <c r="AL32" t="n">
-        <v>52.73763994761728</v>
+        <v>42.67230557956277</v>
       </c>
       <c r="AM32" t="n">
-        <v>14.7827543184902</v>
+        <v>14.51526780295012</v>
       </c>
       <c r="AN32" t="n">
         <v>7.463008588991048</v>
@@ -4800,10 +4800,10 @@
         <v>2.8</v>
       </c>
       <c r="AP32" t="n">
-        <v>53.03300858899106</v>
+        <v>46.71112967666069</v>
       </c>
       <c r="AQ32" t="n">
-        <v>14.63177415120961</v>
+        <v>5.211665590303415</v>
       </c>
       <c r="AR32" t="n">
         <v>7.463008588991048</v>
@@ -4826,10 +4826,10 @@
         <v>2.9</v>
       </c>
       <c r="F33" t="n">
-        <v>78.64204700738138</v>
+        <v>47.49557665558267</v>
       </c>
       <c r="G33" t="n">
-        <v>21.48258971388081</v>
+        <v>17.98705334555375</v>
       </c>
       <c r="H33" t="n">
         <v>6.192775541957416</v>
@@ -4838,10 +4838,10 @@
         <v>2.9</v>
       </c>
       <c r="J33" t="n">
-        <v>72.34339826740192</v>
+        <v>48.2490971947845</v>
       </c>
       <c r="K33" t="n">
-        <v>29.13549443463587</v>
+        <v>10.78153766718663</v>
       </c>
       <c r="L33" t="n">
         <v>6.192775541957416</v>
@@ -4850,10 +4850,10 @@
         <v>2.9</v>
       </c>
       <c r="N33" t="n">
-        <v>48.9476604857425</v>
+        <v>54.6920654056586</v>
       </c>
       <c r="O33" t="n">
-        <v>22.89326601344701</v>
+        <v>14.37196931592702</v>
       </c>
       <c r="P33" t="n">
         <v>6.192775541957416</v>
@@ -4862,10 +4862,10 @@
         <v>2.9</v>
       </c>
       <c r="R33" t="n">
-        <v>49.16706411580214</v>
+        <v>54.60544036502448</v>
       </c>
       <c r="S33" t="n">
-        <v>16.97781317088684</v>
+        <v>11.61551115389327</v>
       </c>
       <c r="T33" t="n">
         <v>6.192775541957416</v>
@@ -4874,10 +4874,10 @@
         <v>2.9</v>
       </c>
       <c r="V33" t="n">
-        <v>60.48764117598375</v>
+        <v>67.16208587292266</v>
       </c>
       <c r="W33" t="n">
-        <v>15.11949995624993</v>
+        <v>22.17868827695036</v>
       </c>
       <c r="X33" t="n">
         <v>6.192775541957416</v>
@@ -4886,10 +4886,10 @@
         <v>2.9</v>
       </c>
       <c r="Z33" t="n">
-        <v>53.49863980352833</v>
+        <v>57.47866259693227</v>
       </c>
       <c r="AA33" t="n">
-        <v>15.79673572398735</v>
+        <v>27.21401604172044</v>
       </c>
       <c r="AB33" t="n">
         <v>6.192775541957416</v>
@@ -4898,10 +4898,10 @@
         <v>2.9</v>
       </c>
       <c r="AD33" t="n">
-        <v>38.52674600486957</v>
+        <v>55.2311715724872</v>
       </c>
       <c r="AE33" t="n">
-        <v>21.44664019246408</v>
+        <v>16.22709506653628</v>
       </c>
       <c r="AF33" t="n">
         <v>6.192775541957416</v>
@@ -4910,10 +4910,10 @@
         <v>2.9</v>
       </c>
       <c r="AH33" t="n">
-        <v>73.02054902587884</v>
+        <v>78.39148708714988</v>
       </c>
       <c r="AI33" t="n">
-        <v>-3.700131734269341</v>
+        <v>3.120037190902111</v>
       </c>
       <c r="AJ33" t="n">
         <v>6.192775541957416</v>
@@ -4922,10 +4922,10 @@
         <v>2.9</v>
       </c>
       <c r="AL33" t="n">
-        <v>54.49198105324847</v>
+        <v>43.64309537795773</v>
       </c>
       <c r="AM33" t="n">
-        <v>15.27734285840691</v>
+        <v>14.99403158120125</v>
       </c>
       <c r="AN33" t="n">
         <v>6.192775541957416</v>
@@ -4934,10 +4934,10 @@
         <v>2.9</v>
       </c>
       <c r="AP33" t="n">
-        <v>54.80077554195743</v>
+        <v>47.9925982517555</v>
       </c>
       <c r="AQ33" t="n">
-        <v>15.11949995624993</v>
+        <v>4.974767659889412</v>
       </c>
       <c r="AR33" t="n">
         <v>6.192775541957416</v>
@@ -4960,10 +4960,10 @@
         <v>3</v>
       </c>
       <c r="F34" t="n">
-        <v>82.11276192216374</v>
+        <v>48.85749922597267</v>
       </c>
       <c r="G34" t="n">
-        <v>22.42482193018047</v>
+        <v>18.63408767222207</v>
       </c>
       <c r="H34" t="n">
         <v>4.824542494923783</v>
@@ -4972,10 +4972,10 @@
         <v>3</v>
       </c>
       <c r="J34" t="n">
-        <v>75.36420970075719</v>
+        <v>49.54888712295281</v>
       </c>
       <c r="K34" t="n">
-        <v>30.62436270241805</v>
+        <v>10.95940902300814</v>
       </c>
       <c r="L34" t="n">
         <v>4.824542494923783</v>
@@ -4984,10 +4984,10 @@
         <v>3</v>
       </c>
       <c r="N34" t="n">
-        <v>50.40736875153966</v>
+        <v>56.45425747984041</v>
       </c>
       <c r="O34" t="n">
-        <v>23.79013740044507</v>
+        <v>14.8213602163354</v>
       </c>
       <c r="P34" t="n">
         <v>4.824542494923783</v>
@@ -4996,10 +4996,10 @@
         <v>3</v>
       </c>
       <c r="R34" t="n">
-        <v>50.53242310975742</v>
+        <v>56.35925480535278</v>
       </c>
       <c r="S34" t="n">
-        <v>17.59827563411551</v>
+        <v>11.85295204447954</v>
       </c>
       <c r="T34" t="n">
         <v>4.824542494923783</v>
@@ -5008,10 +5008,10 @@
         <v>3</v>
       </c>
       <c r="V34" t="n">
-        <v>62.64760575888297</v>
+        <v>69.81280356381512</v>
       </c>
       <c r="W34" t="n">
-        <v>15.60722576129025</v>
+        <v>23.17064181918357</v>
       </c>
       <c r="X34" t="n">
         <v>4.824542494923783</v>
@@ -5020,10 +5020,10 @@
         <v>3</v>
       </c>
       <c r="Z34" t="n">
-        <v>55.17339706089263</v>
+        <v>59.3837570911794</v>
       </c>
       <c r="AA34" t="n">
-        <v>16.33283551243749</v>
+        <v>28.32197344088745</v>
       </c>
       <c r="AB34" t="n">
         <v>4.824542494923783</v>
@@ -5032,10 +5032,10 @@
         <v>3</v>
       </c>
       <c r="AD34" t="n">
-        <v>39.13208227661537</v>
+        <v>57.02968109906283</v>
       </c>
       <c r="AE34" t="n">
-        <v>22.38630458580542</v>
+        <v>16.79393480802562</v>
       </c>
       <c r="AF34" t="n">
         <v>4.824542494923783</v>
@@ -5044,10 +5044,10 @@
         <v>3</v>
       </c>
       <c r="AH34" t="n">
-        <v>76.08972837055387</v>
+        <v>81.84430486477285</v>
       </c>
       <c r="AI34" t="n">
-        <v>-4.556665335694683</v>
+        <v>2.750658512703301</v>
       </c>
       <c r="AJ34" t="n">
         <v>4.824542494923783</v>
@@ -5056,10 +5056,10 @@
         <v>3</v>
       </c>
       <c r="AL34" t="n">
-        <v>56.24632215887967</v>
+        <v>44.61388517635269</v>
       </c>
       <c r="AM34" t="n">
-        <v>15.77193139832362</v>
+        <v>15.47279535945237</v>
       </c>
       <c r="AN34" t="n">
         <v>4.824542494923783</v>
@@ -5068,10 +5068,10 @@
         <v>3</v>
       </c>
       <c r="AP34" t="n">
-        <v>56.5685424949238</v>
+        <v>49.2740668268503</v>
       </c>
       <c r="AQ34" t="n">
-        <v>15.60722576129025</v>
+        <v>4.73786972947541</v>
       </c>
       <c r="AR34" t="n">
         <v>4.824542494923783</v>
@@ -5094,10 +5094,10 @@
         <v>3.1</v>
       </c>
       <c r="F35" t="n">
-        <v>85.5834768369461</v>
+        <v>50.21942179636266</v>
       </c>
       <c r="G35" t="n">
-        <v>23.36705414648014</v>
+        <v>19.28112199889038</v>
       </c>
       <c r="H35" t="n">
         <v>3.35830944789015</v>
@@ -5106,10 +5106,10 @@
         <v>3.1</v>
       </c>
       <c r="J35" t="n">
-        <v>78.38502113411245</v>
+        <v>50.84867705112111</v>
       </c>
       <c r="K35" t="n">
-        <v>32.11323097020022</v>
+        <v>11.13728037882966</v>
       </c>
       <c r="L35" t="n">
         <v>3.35830944789015</v>
@@ -5118,10 +5118,10 @@
         <v>3.1</v>
       </c>
       <c r="N35" t="n">
-        <v>51.86707701733683</v>
+        <v>58.21644955402222</v>
       </c>
       <c r="O35" t="n">
-        <v>24.68700878744313</v>
+        <v>15.27075111674378</v>
       </c>
       <c r="P35" t="n">
         <v>3.35830944789015</v>
@@ -5130,10 +5130,10 @@
         <v>3.1</v>
       </c>
       <c r="R35" t="n">
-        <v>51.89778210371269</v>
+        <v>58.11306924568107</v>
       </c>
       <c r="S35" t="n">
-        <v>18.21873809734418</v>
+        <v>12.09039293506581</v>
       </c>
       <c r="T35" t="n">
         <v>3.35830944789015</v>
@@ -5142,10 +5142,10 @@
         <v>3.1</v>
       </c>
       <c r="V35" t="n">
-        <v>64.8075703417822</v>
+        <v>72.46352125470759</v>
       </c>
       <c r="W35" t="n">
-        <v>16.09495156633057</v>
+        <v>24.16259536141678</v>
       </c>
       <c r="X35" t="n">
         <v>3.35830944789015</v>
@@ -5154,10 +5154,10 @@
         <v>3.1</v>
       </c>
       <c r="Z35" t="n">
-        <v>56.84815431825692</v>
+        <v>61.28885158542653</v>
       </c>
       <c r="AA35" t="n">
-        <v>16.86893530088762</v>
+        <v>29.42993084005447</v>
       </c>
       <c r="AB35" t="n">
         <v>3.35830944789015</v>
@@ -5166,10 +5166,10 @@
         <v>3.1</v>
       </c>
       <c r="AD35" t="n">
-        <v>39.73741854836118</v>
+        <v>58.82819062563847</v>
       </c>
       <c r="AE35" t="n">
-        <v>23.32596897914675</v>
+        <v>17.36077454951497</v>
       </c>
       <c r="AF35" t="n">
         <v>3.35830944789015</v>
@@ -5178,10 +5178,10 @@
         <v>3.1</v>
       </c>
       <c r="AH35" t="n">
-        <v>79.15890771522891</v>
+        <v>85.29712264239582</v>
       </c>
       <c r="AI35" t="n">
-        <v>-5.413198937120026</v>
+        <v>2.381279834504491</v>
       </c>
       <c r="AJ35" t="n">
         <v>3.35830944789015</v>
@@ -5190,10 +5190,10 @@
         <v>3.1</v>
       </c>
       <c r="AL35" t="n">
-        <v>58.00066326451087</v>
+        <v>45.58467497474765</v>
       </c>
       <c r="AM35" t="n">
-        <v>16.26651993824033</v>
+        <v>15.9515591377035</v>
       </c>
       <c r="AN35" t="n">
         <v>3.35830944789015</v>
@@ -5202,10 +5202,10 @@
         <v>3.1</v>
       </c>
       <c r="AP35" t="n">
-        <v>58.33630944789017</v>
+        <v>50.55553540194511</v>
       </c>
       <c r="AQ35" t="n">
-        <v>16.09495156633057</v>
+        <v>4.500971799061407</v>
       </c>
       <c r="AR35" t="n">
         <v>3.35830944789015</v>
@@ -5228,10 +5228,10 @@
         <v>3.2</v>
       </c>
       <c r="F36" t="n">
-        <v>89.05419175172847</v>
+        <v>51.58134436675265</v>
       </c>
       <c r="G36" t="n">
-        <v>24.30928636277981</v>
+        <v>19.92815632555869</v>
       </c>
       <c r="H36" t="n">
         <v>1.794076400856517</v>
@@ -5240,10 +5240,10 @@
         <v>3.2</v>
       </c>
       <c r="J36" t="n">
-        <v>81.40583256746771</v>
+        <v>52.14846697928941</v>
       </c>
       <c r="K36" t="n">
-        <v>33.60209923798239</v>
+        <v>11.31515173465117</v>
       </c>
       <c r="L36" t="n">
         <v>1.794076400856517</v>
@@ -5252,10 +5252,10 @@
         <v>3.2</v>
       </c>
       <c r="N36" t="n">
-        <v>53.32678528313399</v>
+        <v>59.97864162820403</v>
       </c>
       <c r="O36" t="n">
-        <v>25.58388017444119</v>
+        <v>15.72014201715215</v>
       </c>
       <c r="P36" t="n">
         <v>1.794076400856517</v>
@@ -5264,10 +5264,10 @@
         <v>3.2</v>
       </c>
       <c r="R36" t="n">
-        <v>53.26314109766797</v>
+        <v>59.86688368600937</v>
       </c>
       <c r="S36" t="n">
-        <v>18.83920056057285</v>
+        <v>12.32783382565209</v>
       </c>
       <c r="T36" t="n">
         <v>1.794076400856517</v>
@@ -5276,10 +5276,10 @@
         <v>3.2</v>
       </c>
       <c r="V36" t="n">
-        <v>66.96753492468142</v>
+        <v>75.11423894560005</v>
       </c>
       <c r="W36" t="n">
-        <v>16.58267737137089</v>
+        <v>25.15454890364999</v>
       </c>
       <c r="X36" t="n">
         <v>1.794076400856517</v>
@@ -5288,10 +5288,10 @@
         <v>3.2</v>
       </c>
       <c r="Z36" t="n">
-        <v>58.52291157562121</v>
+        <v>63.19394607967366</v>
       </c>
       <c r="AA36" t="n">
-        <v>17.40503508933776</v>
+        <v>30.53788823922148</v>
       </c>
       <c r="AB36" t="n">
         <v>1.794076400856517</v>
@@ -5300,10 +5300,10 @@
         <v>3.2</v>
       </c>
       <c r="AD36" t="n">
-        <v>40.34275482010698</v>
+        <v>60.62670015221411</v>
       </c>
       <c r="AE36" t="n">
-        <v>24.26563337248808</v>
+        <v>17.92761429100431</v>
       </c>
       <c r="AF36" t="n">
         <v>1.794076400856517</v>
@@ -5312,10 +5312,10 @@
         <v>3.2</v>
       </c>
       <c r="AH36" t="n">
-        <v>82.22808705990394</v>
+        <v>88.74994042001879</v>
       </c>
       <c r="AI36" t="n">
-        <v>-6.269732538545368</v>
+        <v>2.01190115630568</v>
       </c>
       <c r="AJ36" t="n">
         <v>1.794076400856517</v>
@@ -5324,10 +5324,10 @@
         <v>3.2</v>
       </c>
       <c r="AL36" t="n">
-        <v>59.75500437014207</v>
+        <v>46.55546477314261</v>
       </c>
       <c r="AM36" t="n">
-        <v>16.76110847815704</v>
+        <v>16.43032291595463</v>
       </c>
       <c r="AN36" t="n">
         <v>1.794076400856517</v>
@@ -5336,10 +5336,10 @@
         <v>3.2</v>
       </c>
       <c r="AP36" t="n">
-        <v>60.10407640085653</v>
+        <v>51.83700397703991</v>
       </c>
       <c r="AQ36" t="n">
-        <v>16.58267737137089</v>
+        <v>4.264073868647404</v>
       </c>
       <c r="AR36" t="n">
         <v>1.794076400856517</v>
@@ -5362,10 +5362,10 @@
         <v>3.3</v>
       </c>
       <c r="F37" t="n">
-        <v>92.52490666651083</v>
+        <v>52.94326693714265</v>
       </c>
       <c r="G37" t="n">
-        <v>25.25151857907948</v>
+        <v>20.575190652227</v>
       </c>
       <c r="H37" t="n">
         <v>0.1318433538228847</v>
@@ -5374,10 +5374,10 @@
         <v>3.3</v>
       </c>
       <c r="J37" t="n">
-        <v>84.42664400082298</v>
+        <v>53.44825690745771</v>
       </c>
       <c r="K37" t="n">
-        <v>35.09096750576457</v>
+        <v>11.49302309047268</v>
       </c>
       <c r="L37" t="n">
         <v>0.1318433538228847</v>
@@ -5386,10 +5386,10 @@
         <v>3.3</v>
       </c>
       <c r="N37" t="n">
-        <v>54.78649354893115</v>
+        <v>61.74083370238584</v>
       </c>
       <c r="O37" t="n">
-        <v>26.48075156143925</v>
+        <v>16.16953291756053</v>
       </c>
       <c r="P37" t="n">
         <v>0.1318433538228847</v>
@@ -5398,10 +5398,10 @@
         <v>3.3</v>
       </c>
       <c r="R37" t="n">
-        <v>54.62850009162324</v>
+        <v>61.62069812633767</v>
       </c>
       <c r="S37" t="n">
-        <v>19.45966302380152</v>
+        <v>12.56527471623836</v>
       </c>
       <c r="T37" t="n">
         <v>0.1318433538228847</v>
@@ -5410,10 +5410,10 @@
         <v>3.3</v>
       </c>
       <c r="V37" t="n">
-        <v>69.12749950758064</v>
+        <v>77.76495663649251</v>
       </c>
       <c r="W37" t="n">
-        <v>17.07040317641121</v>
+        <v>26.14650244588319</v>
       </c>
       <c r="X37" t="n">
         <v>0.1318433538228847</v>
@@ -5422,10 +5422,10 @@
         <v>3.3</v>
       </c>
       <c r="Z37" t="n">
-        <v>60.1976688329855</v>
+        <v>65.09904057392079</v>
       </c>
       <c r="AA37" t="n">
-        <v>17.9411348777879</v>
+        <v>31.64584563838849</v>
       </c>
       <c r="AB37" t="n">
         <v>0.1318433538228847</v>
@@ -5434,10 +5434,10 @@
         <v>3.3</v>
       </c>
       <c r="AD37" t="n">
-        <v>40.94809109185279</v>
+        <v>62.42520967878974</v>
       </c>
       <c r="AE37" t="n">
-        <v>25.20529776582941</v>
+        <v>18.49445403249366</v>
       </c>
       <c r="AF37" t="n">
         <v>0.1318433538228847</v>
@@ -5446,10 +5446,10 @@
         <v>3.3</v>
       </c>
       <c r="AH37" t="n">
-        <v>85.29726640457898</v>
+        <v>92.20275819764176</v>
       </c>
       <c r="AI37" t="n">
-        <v>-7.12626613997071</v>
+        <v>1.64252247810687</v>
       </c>
       <c r="AJ37" t="n">
         <v>0.1318433538228847</v>
@@ -5458,10 +5458,10 @@
         <v>3.3</v>
       </c>
       <c r="AL37" t="n">
-        <v>61.50934547577327</v>
+        <v>47.52625457153757</v>
       </c>
       <c r="AM37" t="n">
-        <v>17.25569701807375</v>
+        <v>16.90908669420576</v>
       </c>
       <c r="AN37" t="n">
         <v>0.1318433538228847</v>
@@ -5470,10 +5470,10 @@
         <v>3.3</v>
       </c>
       <c r="AP37" t="n">
-        <v>61.8718433538229</v>
+        <v>53.11847255213472</v>
       </c>
       <c r="AQ37" t="n">
-        <v>17.07040317641121</v>
+        <v>4.027175938233402</v>
       </c>
       <c r="AR37" t="n">
         <v>0.1318433538228847</v>

</xml_diff>